<commit_message>
forgot to update the bondpad cells
</commit_message>
<xml_diff>
--- a/masks/code/TKIDModule_spreadsheet_20200602_AW_CF.xlsx
+++ b/masks/code/TKIDModule_spreadsheet_20200602_AW_CF.xlsx
@@ -1050,7 +1050,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1114,6 +1114,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1439,8 +1443,8 @@
   <dimension ref="A4:AC157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S100" sqref="S100"/>
+      <pane ySplit="14" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S124" sqref="S124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1779,18 +1783,18 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="29" t="s">
+      <c r="T12" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="29" t="s">
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="AA12" s="30"/>
+      <c r="AA12" s="32"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
@@ -1798,50 +1802,50 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="29" t="s">
+      <c r="E13" s="32"/>
+      <c r="F13" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="29" t="s">
+      <c r="G13" s="32"/>
+      <c r="H13" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="29" t="s">
+      <c r="M13" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="30"/>
-      <c r="O13" s="29" t="s">
+      <c r="N13" s="32"/>
+      <c r="O13" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="P13" s="30"/>
+      <c r="P13" s="32"/>
       <c r="Q13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="29" t="s">
+      <c r="T13" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="U13" s="30"/>
-      <c r="V13" s="29" t="s">
+      <c r="U13" s="32"/>
+      <c r="V13" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="W13" s="30"/>
-      <c r="X13" s="29" t="s">
+      <c r="W13" s="32"/>
+      <c r="X13" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="29" t="s">
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="AA13" s="30"/>
+      <c r="AA13" s="32"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
     </row>
@@ -3688,151 +3692,149 @@
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="29"/>
+      <c r="C39" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="29">
         <v>-2.6</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="29">
         <v>-3.9</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="29">
         <v>0.9</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="29">
         <v>0.9</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="29">
         <v>-3.05</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="29">
         <v>-2.15</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="29">
         <v>-3.45</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K39" s="29">
         <v>-4.3499999999999996</v>
       </c>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1">
-        <v>0</v>
-      </c>
-      <c r="N39" s="1">
-        <v>0</v>
-      </c>
-      <c r="O39" s="1">
+      <c r="L39" s="29"/>
+      <c r="M39" s="29">
+        <v>0</v>
+      </c>
+      <c r="N39" s="29">
+        <v>0</v>
+      </c>
+      <c r="O39" s="29">
         <v>-2.6</v>
       </c>
-      <c r="P39" s="1">
+      <c r="P39" s="29">
         <v>-3.9</v>
       </c>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1" t="s">
+      <c r="Q39" s="29"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="T39" s="1">
-        <v>9</v>
-      </c>
-      <c r="U39" s="1">
-        <v>1</v>
-      </c>
-      <c r="V39" s="1">
-        <v>13.5</v>
-      </c>
-      <c r="W39" s="1">
+      <c r="T39" s="29">
+        <v>11</v>
+      </c>
+      <c r="U39" s="29">
+        <v>1</v>
+      </c>
+      <c r="V39" s="29">
+        <v>14.5</v>
+      </c>
+      <c r="W39" s="29">
         <v>35.945</v>
       </c>
-      <c r="X39" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y39" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-      <c r="AB39" s="1"/>
-      <c r="AC39" s="1"/>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
+      <c r="X39" s="29">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="29">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="29"/>
+    </row>
+    <row r="40" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1" t="s">
+      <c r="B40" s="29"/>
+      <c r="C40" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="29">
         <v>-2.6</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="29">
         <v>-3.9</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="29">
         <v>0.9</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="29">
         <v>0.9</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="29">
         <v>-3.05</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="29">
         <v>-2.15</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J40" s="29">
         <v>-3.45</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="29">
         <v>-4.3499999999999996</v>
       </c>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1">
-        <v>0</v>
-      </c>
-      <c r="N40" s="1">
-        <v>0</v>
-      </c>
-      <c r="O40" s="1">
+      <c r="L40" s="29"/>
+      <c r="M40" s="29">
+        <v>0</v>
+      </c>
+      <c r="N40" s="29">
+        <v>0</v>
+      </c>
+      <c r="O40" s="29">
         <v>-2.6</v>
       </c>
-      <c r="P40" s="1">
+      <c r="P40" s="29">
         <v>-3.9</v>
       </c>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1" t="s">
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="T40" s="1">
-        <v>9</v>
-      </c>
-      <c r="U40" s="1">
-        <v>1</v>
-      </c>
-      <c r="V40" s="1">
-        <v>-21.2</v>
-      </c>
-      <c r="W40" s="1">
+      <c r="T40" s="29">
+        <v>11</v>
+      </c>
+      <c r="U40" s="29">
+        <v>1</v>
+      </c>
+      <c r="V40" s="29">
+        <v>-22.2</v>
+      </c>
+      <c r="W40" s="29">
         <v>35.945</v>
       </c>
-      <c r="X40" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y40" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="1"/>
-      <c r="AA40" s="1"/>
-      <c r="AB40" s="1"/>
-      <c r="AC40" s="1"/>
+      <c r="X40" s="29">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="29">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="29"/>
+      <c r="AB40" s="29"/>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
@@ -9780,151 +9782,149 @@
         <v>283</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A122" s="1" t="s">
+    <row r="122" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A122" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1" t="s">
+      <c r="B122" s="29"/>
+      <c r="C122" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="D122" s="1">
+      <c r="D122" s="29">
         <v>-1.65</v>
       </c>
-      <c r="E122" s="1">
+      <c r="E122" s="29">
         <v>-3.9</v>
       </c>
-      <c r="F122" s="1">
+      <c r="F122" s="29">
         <v>0.9</v>
       </c>
-      <c r="G122" s="1">
+      <c r="G122" s="29">
         <v>0.9</v>
       </c>
-      <c r="H122" s="1">
+      <c r="H122" s="29">
         <v>-2.1</v>
       </c>
-      <c r="I122" s="1">
+      <c r="I122" s="29">
         <v>-1.2</v>
       </c>
-      <c r="J122" s="1">
+      <c r="J122" s="29">
         <v>-3.45</v>
       </c>
-      <c r="K122" s="1">
+      <c r="K122" s="29">
         <v>-4.3499999999999996</v>
       </c>
-      <c r="L122" s="1"/>
-      <c r="M122" s="1">
-        <v>0</v>
-      </c>
-      <c r="N122" s="1">
-        <v>0</v>
-      </c>
-      <c r="O122" s="1">
+      <c r="L122" s="29"/>
+      <c r="M122" s="29">
+        <v>0</v>
+      </c>
+      <c r="N122" s="29">
+        <v>0</v>
+      </c>
+      <c r="O122" s="29">
         <v>-1.65</v>
       </c>
-      <c r="P122" s="1">
+      <c r="P122" s="29">
         <v>-3.9</v>
       </c>
-      <c r="Q122" s="1"/>
-      <c r="R122" s="1"/>
-      <c r="S122" s="1" t="s">
+      <c r="Q122" s="29"/>
+      <c r="R122" s="29"/>
+      <c r="S122" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="T122" s="1">
-        <v>9</v>
-      </c>
-      <c r="U122" s="1">
-        <v>1</v>
-      </c>
-      <c r="V122" s="1">
-        <v>13.5</v>
-      </c>
-      <c r="W122" s="1">
+      <c r="T122" s="29">
+        <v>11</v>
+      </c>
+      <c r="U122" s="29">
+        <v>1</v>
+      </c>
+      <c r="V122" s="29">
+        <v>14.5</v>
+      </c>
+      <c r="W122" s="29">
         <v>35.945</v>
       </c>
-      <c r="X122" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y122" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z122" s="1"/>
-      <c r="AA122" s="1"/>
-      <c r="AB122" s="1"/>
-      <c r="AC122" s="1"/>
-    </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A123" s="1" t="s">
+      <c r="X122" s="29">
+        <v>1</v>
+      </c>
+      <c r="Y122" s="29">
+        <v>0</v>
+      </c>
+      <c r="Z122" s="29"/>
+      <c r="AA122" s="29"/>
+      <c r="AB122" s="29"/>
+    </row>
+    <row r="123" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A123" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1" t="s">
+      <c r="B123" s="29"/>
+      <c r="C123" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="D123" s="1">
+      <c r="D123" s="29">
         <v>-1.65</v>
       </c>
-      <c r="E123" s="1">
+      <c r="E123" s="29">
         <v>-3.9</v>
       </c>
-      <c r="F123" s="1">
+      <c r="F123" s="29">
         <v>0.9</v>
       </c>
-      <c r="G123" s="1">
+      <c r="G123" s="29">
         <v>0.9</v>
       </c>
-      <c r="H123" s="1">
+      <c r="H123" s="29">
         <v>-2.1</v>
       </c>
-      <c r="I123" s="1">
+      <c r="I123" s="29">
         <v>-1.2</v>
       </c>
-      <c r="J123" s="1">
+      <c r="J123" s="29">
         <v>-3.45</v>
       </c>
-      <c r="K123" s="1">
+      <c r="K123" s="29">
         <v>-4.3499999999999996</v>
       </c>
-      <c r="L123" s="1"/>
-      <c r="M123" s="1">
-        <v>0</v>
-      </c>
-      <c r="N123" s="1">
-        <v>0</v>
-      </c>
-      <c r="O123" s="1">
+      <c r="L123" s="29"/>
+      <c r="M123" s="29">
+        <v>0</v>
+      </c>
+      <c r="N123" s="29">
+        <v>0</v>
+      </c>
+      <c r="O123" s="29">
         <v>-1.65</v>
       </c>
-      <c r="P123" s="1">
+      <c r="P123" s="29">
         <v>-3.9</v>
       </c>
-      <c r="Q123" s="1"/>
-      <c r="R123" s="1"/>
-      <c r="S123" s="1" t="s">
+      <c r="Q123" s="29"/>
+      <c r="R123" s="29"/>
+      <c r="S123" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="T123" s="1">
-        <v>9</v>
-      </c>
-      <c r="U123" s="1">
-        <v>1</v>
-      </c>
-      <c r="V123" s="1">
-        <v>-21.2</v>
-      </c>
-      <c r="W123" s="1">
+      <c r="T123" s="29">
+        <v>11</v>
+      </c>
+      <c r="U123" s="29">
+        <v>1</v>
+      </c>
+      <c r="V123" s="29">
+        <v>-22.2</v>
+      </c>
+      <c r="W123" s="29">
         <v>35.945</v>
       </c>
-      <c r="X123" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y123" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z123" s="1"/>
-      <c r="AA123" s="1"/>
-      <c r="AB123" s="1"/>
-      <c r="AC123" s="1"/>
+      <c r="X123" s="29">
+        <v>1</v>
+      </c>
+      <c r="Y123" s="29">
+        <v>0</v>
+      </c>
+      <c r="Z123" s="29"/>
+      <c r="AA123" s="29"/>
+      <c r="AB123" s="29"/>
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A124" s="1" t="s">
@@ -12390,17 +12390,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="O13:P13"/>
     <mergeCell ref="T12:Y12"/>
     <mergeCell ref="T13:U13"/>
     <mergeCell ref="V13:W13"/>
     <mergeCell ref="X13:Y13"/>
     <mergeCell ref="Z12:AA12"/>
     <mergeCell ref="Z13:AA13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="O13:P13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -12441,18 +12441,18 @@
       <c r="A1" s="3"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="29" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="31" t="s">
         <v>268</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="29" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="31" t="s">
         <v>269</v>
       </c>
-      <c r="I1" s="30"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
         <v>270</v>
@@ -28616,18 +28616,18 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
-      <c r="T1" s="29" t="s">
+      <c r="T1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="29" t="s">
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="30"/>
+      <c r="AA1" s="32"/>
       <c r="AB1" s="1"/>
       <c r="AE1" s="15"/>
       <c r="AF1" s="16"/>
@@ -28637,10 +28637,10 @@
       <c r="AJ1" s="16"/>
       <c r="AK1" s="16"/>
       <c r="AL1" s="16"/>
-      <c r="AM1" s="31" t="s">
+      <c r="AM1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="AN1" s="32"/>
+      <c r="AN1" s="34"/>
       <c r="AO1" s="16"/>
       <c r="AP1" s="18"/>
       <c r="AQ1" s="18"/>
@@ -28651,74 +28651,74 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="29" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="29" t="s">
+      <c r="N2" s="32"/>
+      <c r="O2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="30"/>
+      <c r="P2" s="32"/>
       <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="29" t="s">
+      <c r="T2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="30"/>
-      <c r="V2" s="29" t="s">
+      <c r="U2" s="32"/>
+      <c r="V2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="30"/>
-      <c r="X2" s="29" t="s">
+      <c r="W2" s="32"/>
+      <c r="X2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="29" t="s">
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="AA2" s="30"/>
+      <c r="AA2" s="32"/>
       <c r="AB2" s="1"/>
       <c r="AE2" s="15"/>
       <c r="AF2" s="16"/>
-      <c r="AG2" s="31" t="s">
+      <c r="AG2" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
       <c r="AK2" s="16"/>
       <c r="AL2" s="16"/>
-      <c r="AM2" s="31" t="s">
+      <c r="AM2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AN2" s="32"/>
+      <c r="AN2" s="34"/>
       <c r="AO2" s="16"/>
-      <c r="AP2" s="33" t="s">
+      <c r="AP2" s="35" t="s">
         <v>289</v>
       </c>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="33" t="s">
+      <c r="AQ2" s="36"/>
+      <c r="AR2" s="35" t="s">
         <v>290</v>
       </c>
-      <c r="AS2" s="34"/>
+      <c r="AS2" s="36"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -43490,11 +43490,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AG2:AJ2"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AR2:AS2"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="T1:Y1"/>
     <mergeCell ref="Z1:AA1"/>
@@ -43506,6 +43501,11 @@
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="AG2:AJ2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AR2:AS2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the gp edge opening and filler cells
</commit_message>
<xml_diff>
--- a/masks/code/TKIDModule_spreadsheet_20200602_AW_CF.xlsx
+++ b/masks/code/TKIDModule_spreadsheet_20200602_AW_CF.xlsx
@@ -938,7 +938,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -954,6 +954,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1050,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1118,14 +1124,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1137,6 +1135,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1443,8 +1445,8 @@
   <dimension ref="A4:AC157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S124" sqref="S124"/>
+      <pane ySplit="14" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S67" sqref="S67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1783,18 +1785,18 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="31" t="s">
+      <c r="T12" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="U12" s="32"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="31" t="s">
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AA12" s="32"/>
+      <c r="AA12" s="28"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
     </row>
@@ -1802,50 +1804,50 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="31" t="s">
+      <c r="E13" s="28"/>
+      <c r="F13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="31" t="s">
+      <c r="G13" s="28"/>
+      <c r="H13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="31" t="s">
+      <c r="M13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="32"/>
-      <c r="O13" s="31" t="s">
+      <c r="N13" s="28"/>
+      <c r="O13" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="P13" s="32"/>
+      <c r="P13" s="28"/>
       <c r="Q13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="31" t="s">
+      <c r="T13" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="U13" s="32"/>
-      <c r="V13" s="31" t="s">
+      <c r="U13" s="28"/>
+      <c r="V13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="W13" s="32"/>
-      <c r="X13" s="31" t="s">
+      <c r="W13" s="28"/>
+      <c r="X13" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="31" t="s">
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AA13" s="32"/>
+      <c r="AA13" s="28"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
     </row>
@@ -3692,149 +3694,149 @@
       <c r="AB38" s="1"/>
       <c r="AC38" s="1"/>
     </row>
-    <row r="39" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="29" t="s">
+    <row r="39" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A39" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29" t="s">
+      <c r="B39" s="34"/>
+      <c r="C39" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39" s="34">
         <v>-2.6</v>
       </c>
-      <c r="E39" s="29">
+      <c r="E39" s="34">
         <v>-3.9</v>
       </c>
-      <c r="F39" s="29">
+      <c r="F39" s="34">
         <v>0.9</v>
       </c>
-      <c r="G39" s="29">
+      <c r="G39" s="34">
         <v>0.9</v>
       </c>
-      <c r="H39" s="29">
+      <c r="H39" s="34">
         <v>-3.05</v>
       </c>
-      <c r="I39" s="29">
+      <c r="I39" s="34">
         <v>-2.15</v>
       </c>
-      <c r="J39" s="29">
+      <c r="J39" s="34">
         <v>-3.45</v>
       </c>
-      <c r="K39" s="29">
+      <c r="K39" s="34">
         <v>-4.3499999999999996</v>
       </c>
-      <c r="L39" s="29"/>
-      <c r="M39" s="29">
-        <v>0</v>
-      </c>
-      <c r="N39" s="29">
-        <v>0</v>
-      </c>
-      <c r="O39" s="29">
+      <c r="L39" s="34"/>
+      <c r="M39" s="34">
+        <v>0</v>
+      </c>
+      <c r="N39" s="34">
+        <v>0</v>
+      </c>
+      <c r="O39" s="34">
         <v>-2.6</v>
       </c>
-      <c r="P39" s="29">
+      <c r="P39" s="34">
         <v>-3.9</v>
       </c>
-      <c r="Q39" s="29"/>
-      <c r="R39" s="29"/>
-      <c r="S39" s="29" t="s">
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T39" s="29">
+      <c r="T39" s="34">
         <v>11</v>
       </c>
-      <c r="U39" s="29">
-        <v>1</v>
-      </c>
-      <c r="V39" s="29">
+      <c r="U39" s="34">
+        <v>1</v>
+      </c>
+      <c r="V39" s="34">
         <v>14.5</v>
       </c>
-      <c r="W39" s="29">
+      <c r="W39" s="34">
         <v>35.945</v>
       </c>
-      <c r="X39" s="29">
-        <v>1</v>
-      </c>
-      <c r="Y39" s="29">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="29"/>
-      <c r="AA39" s="29"/>
-      <c r="AB39" s="29"/>
-    </row>
-    <row r="40" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="29" t="s">
+      <c r="X39" s="34">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="34"/>
+      <c r="AA39" s="34"/>
+      <c r="AB39" s="34"/>
+    </row>
+    <row r="40" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29" t="s">
+      <c r="B40" s="34"/>
+      <c r="C40" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40" s="34">
         <v>-2.6</v>
       </c>
-      <c r="E40" s="29">
+      <c r="E40" s="34">
         <v>-3.9</v>
       </c>
-      <c r="F40" s="29">
+      <c r="F40" s="34">
         <v>0.9</v>
       </c>
-      <c r="G40" s="29">
+      <c r="G40" s="34">
         <v>0.9</v>
       </c>
-      <c r="H40" s="29">
+      <c r="H40" s="34">
         <v>-3.05</v>
       </c>
-      <c r="I40" s="29">
+      <c r="I40" s="34">
         <v>-2.15</v>
       </c>
-      <c r="J40" s="29">
+      <c r="J40" s="34">
         <v>-3.45</v>
       </c>
-      <c r="K40" s="29">
+      <c r="K40" s="34">
         <v>-4.3499999999999996</v>
       </c>
-      <c r="L40" s="29"/>
-      <c r="M40" s="29">
-        <v>0</v>
-      </c>
-      <c r="N40" s="29">
-        <v>0</v>
-      </c>
-      <c r="O40" s="29">
+      <c r="L40" s="34"/>
+      <c r="M40" s="34">
+        <v>0</v>
+      </c>
+      <c r="N40" s="34">
+        <v>0</v>
+      </c>
+      <c r="O40" s="34">
         <v>-2.6</v>
       </c>
-      <c r="P40" s="29">
+      <c r="P40" s="34">
         <v>-3.9</v>
       </c>
-      <c r="Q40" s="29"/>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29" t="s">
+      <c r="Q40" s="34"/>
+      <c r="R40" s="34"/>
+      <c r="S40" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T40" s="29">
+      <c r="T40" s="34">
         <v>11</v>
       </c>
-      <c r="U40" s="29">
-        <v>1</v>
-      </c>
-      <c r="V40" s="29">
+      <c r="U40" s="34">
+        <v>1</v>
+      </c>
+      <c r="V40" s="34">
         <v>-22.2</v>
       </c>
-      <c r="W40" s="29">
+      <c r="W40" s="34">
         <v>35.945</v>
       </c>
-      <c r="X40" s="29">
-        <v>1</v>
-      </c>
-      <c r="Y40" s="29">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="29"/>
-      <c r="AA40" s="29"/>
-      <c r="AB40" s="29"/>
+      <c r="X40" s="34">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="34"/>
+      <c r="AA40" s="34"/>
+      <c r="AB40" s="34"/>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
@@ -4061,44 +4063,44 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D44" s="1">
-        <v>-3.45</v>
+        <v>-7.55</v>
       </c>
       <c r="E44" s="1">
-        <v>-9.625</v>
+        <v>-2.6190000000000002</v>
       </c>
       <c r="F44" s="1">
-        <v>9.9</v>
+        <v>1.2</v>
       </c>
       <c r="G44" s="1">
-        <v>1.3</v>
+        <v>3.2</v>
       </c>
       <c r="H44" s="1">
-        <v>-8.4</v>
+        <v>-8.15</v>
       </c>
       <c r="I44" s="1">
-        <v>1.5</v>
+        <v>-6.95</v>
       </c>
       <c r="J44" s="1">
-        <v>-8.9749999999999996</v>
+        <v>-1.0189999999999999</v>
       </c>
       <c r="K44" s="1">
-        <v>-10.275</v>
+        <v>-4.2190000000000003</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1">
         <v>0</v>
       </c>
       <c r="N44" s="1">
-        <v>0</v>
+        <v>-1.2999999999999999E-2</v>
       </c>
       <c r="O44" s="1">
-        <v>-3.45</v>
+        <v>-7.55</v>
       </c>
       <c r="P44" s="1">
-        <v>-9.625</v>
+        <v>-2.6059999999999999</v>
       </c>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -4106,27 +4108,31 @@
         <v>32</v>
       </c>
       <c r="T44" s="1">
+        <v>9</v>
+      </c>
+      <c r="U44" s="1">
+        <v>16</v>
+      </c>
+      <c r="V44" s="1">
+        <v>0</v>
+      </c>
+      <c r="W44" s="1">
+        <v>-0.32800000000000001</v>
+      </c>
+      <c r="X44" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="Y44" s="1">
         <v>4</v>
-      </c>
-      <c r="U44" s="1">
-        <v>2</v>
-      </c>
-      <c r="V44" s="1">
-        <v>-3.85</v>
-      </c>
-      <c r="W44" s="1">
-        <v>0</v>
-      </c>
-      <c r="X44" s="1">
-        <v>6.4</v>
-      </c>
-      <c r="Y44" s="1">
-        <v>71.290000000000006</v>
       </c>
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
-      <c r="AB44" s="1"/>
-      <c r="AC44" s="1"/>
+      <c r="AB44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC44" s="1" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
@@ -4134,44 +4140,44 @@
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D45" s="1">
-        <v>-7.55</v>
+        <v>8.5</v>
       </c>
       <c r="E45" s="1">
-        <v>-2.6190000000000002</v>
+        <v>-2.25</v>
       </c>
       <c r="F45" s="1">
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
       <c r="G45" s="1">
-        <v>3.2</v>
+        <v>0.6</v>
       </c>
       <c r="H45" s="1">
-        <v>-8.15</v>
+        <v>8.15</v>
       </c>
       <c r="I45" s="1">
-        <v>-6.95</v>
+        <v>8.85</v>
       </c>
       <c r="J45" s="1">
-        <v>-1.0189999999999999</v>
+        <v>-1.95</v>
       </c>
       <c r="K45" s="1">
-        <v>-4.2190000000000003</v>
+        <v>-2.5499999999999998</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1">
-        <v>0</v>
+        <v>-2.7010000000000001</v>
       </c>
       <c r="N45" s="1">
-        <v>-1.2999999999999999E-2</v>
+        <v>-3.9860000000000002</v>
       </c>
       <c r="O45" s="1">
-        <v>-7.55</v>
+        <v>11.201000000000001</v>
       </c>
       <c r="P45" s="1">
-        <v>-2.6059999999999999</v>
+        <v>1.736</v>
       </c>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -4179,31 +4185,27 @@
         <v>32</v>
       </c>
       <c r="T45" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="U45" s="1">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="V45" s="1">
-        <v>0</v>
+        <v>-29.4</v>
       </c>
       <c r="W45" s="1">
-        <v>-0.32800000000000001</v>
+        <v>-4.5419999999999998</v>
       </c>
       <c r="X45" s="1">
-        <v>8.4</v>
+        <v>0</v>
       </c>
       <c r="Y45" s="1">
-        <v>4</v>
+        <v>16.8</v>
       </c>
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
-      <c r="AB45" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC45" s="1" t="s">
-        <v>286</v>
-      </c>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1"/>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
@@ -4239,16 +4241,16 @@
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1">
-        <v>-2.7010000000000001</v>
+        <v>2.7050000000000001</v>
       </c>
       <c r="N46" s="1">
-        <v>-3.9860000000000002</v>
+        <v>3.988</v>
       </c>
       <c r="O46" s="1">
-        <v>11.201000000000001</v>
+        <v>5.7949999999999999</v>
       </c>
       <c r="P46" s="1">
-        <v>1.736</v>
+        <v>-6.2380000000000004</v>
       </c>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -4262,7 +4264,7 @@
         <v>3</v>
       </c>
       <c r="V46" s="1">
-        <v>-29.4</v>
+        <v>29.4</v>
       </c>
       <c r="W46" s="1">
         <v>-4.5419999999999998</v>
@@ -4312,16 +4314,16 @@
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1">
-        <v>2.7050000000000001</v>
+        <v>0</v>
       </c>
       <c r="N47" s="1">
-        <v>3.988</v>
+        <v>0</v>
       </c>
       <c r="O47" s="1">
-        <v>5.7949999999999999</v>
+        <v>8.5</v>
       </c>
       <c r="P47" s="1">
-        <v>-6.2380000000000004</v>
+        <v>-2.25</v>
       </c>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
@@ -4332,19 +4334,19 @@
         <v>1</v>
       </c>
       <c r="U47" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V47" s="1">
-        <v>29.4</v>
+        <v>23.704999999999998</v>
       </c>
       <c r="W47" s="1">
-        <v>-4.5419999999999998</v>
+        <v>-33.728000000000002</v>
       </c>
       <c r="X47" s="1">
         <v>0</v>
       </c>
       <c r="Y47" s="1">
-        <v>16.8</v>
+        <v>0</v>
       </c>
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
@@ -4357,31 +4359,31 @@
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D48" s="1">
-        <v>8.5</v>
+        <v>4.83</v>
       </c>
       <c r="E48" s="1">
-        <v>-2.25</v>
+        <v>-8.2200000000000006</v>
       </c>
       <c r="F48" s="1">
-        <v>0.7</v>
+        <v>1.44</v>
       </c>
       <c r="G48" s="1">
-        <v>0.6</v>
+        <v>1.44</v>
       </c>
       <c r="H48" s="1">
-        <v>8.15</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="I48" s="1">
-        <v>8.85</v>
+        <v>5.55</v>
       </c>
       <c r="J48" s="1">
-        <v>-1.95</v>
+        <v>-7.5000000000000009</v>
       </c>
       <c r="K48" s="1">
-        <v>-2.5499999999999998</v>
+        <v>-8.9400000000000013</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1">
@@ -4391,10 +4393,10 @@
         <v>0</v>
       </c>
       <c r="O48" s="1">
-        <v>8.5</v>
+        <v>4.83</v>
       </c>
       <c r="P48" s="1">
-        <v>-2.25</v>
+        <v>-8.2200000000000006</v>
       </c>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
@@ -4402,22 +4404,22 @@
         <v>32</v>
       </c>
       <c r="T48" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U48" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V48" s="1">
-        <v>23.704999999999998</v>
+        <v>0</v>
       </c>
       <c r="W48" s="1">
-        <v>-33.728000000000002</v>
+        <v>6.1029999999999998</v>
       </c>
       <c r="X48" s="1">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="Y48" s="1">
-        <v>0</v>
+        <v>50.472499999999997</v>
       </c>
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
@@ -4430,31 +4432,31 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D49" s="1">
-        <v>4.83</v>
+        <v>-6.4</v>
       </c>
       <c r="E49" s="1">
-        <v>-8.2200000000000006</v>
+        <v>4.2</v>
       </c>
       <c r="F49" s="1">
-        <v>1.44</v>
+        <v>1</v>
       </c>
       <c r="G49" s="1">
-        <v>1.44</v>
+        <v>2.4</v>
       </c>
       <c r="H49" s="1">
-        <v>4.1100000000000003</v>
+        <v>-6.9</v>
       </c>
       <c r="I49" s="1">
-        <v>5.55</v>
+        <v>-5.9</v>
       </c>
       <c r="J49" s="1">
-        <v>-7.5000000000000009</v>
+        <v>5.4</v>
       </c>
       <c r="K49" s="1">
-        <v>-8.9400000000000013</v>
+        <v>3</v>
       </c>
       <c r="L49" s="1"/>
       <c r="M49" s="1">
@@ -4464,10 +4466,10 @@
         <v>0</v>
       </c>
       <c r="O49" s="1">
-        <v>4.83</v>
+        <v>-6.4</v>
       </c>
       <c r="P49" s="1">
-        <v>-8.2200000000000006</v>
+        <v>4.2</v>
       </c>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
@@ -4475,22 +4477,22 @@
         <v>32</v>
       </c>
       <c r="T49" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U49" s="1">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="V49" s="1">
-        <v>0</v>
+        <v>-36.32</v>
       </c>
       <c r="W49" s="1">
-        <v>6.1029999999999998</v>
+        <v>-2.8079999999999998</v>
       </c>
       <c r="X49" s="1">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="Y49" s="1">
-        <v>50.472499999999997</v>
+        <v>1.9950000000000001</v>
       </c>
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
@@ -4503,44 +4505,44 @@
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D50" s="1">
-        <v>-6.4</v>
+        <v>4.54</v>
       </c>
       <c r="E50" s="1">
-        <v>4.2</v>
+        <v>-2.9860000000000002</v>
       </c>
       <c r="F50" s="1">
-        <v>1</v>
+        <v>8.6199999999999992</v>
       </c>
       <c r="G50" s="1">
-        <v>2.4</v>
+        <v>0.8</v>
       </c>
       <c r="H50" s="1">
-        <v>-6.9</v>
+        <v>0.2300000000000004</v>
       </c>
       <c r="I50" s="1">
-        <v>-5.9</v>
+        <v>8.85</v>
       </c>
       <c r="J50" s="1">
-        <v>5.4</v>
+        <v>-2.6</v>
       </c>
       <c r="K50" s="1">
-        <v>3</v>
+        <v>-3.4</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="1">
         <v>0</v>
       </c>
       <c r="N50" s="1">
-        <v>0</v>
+        <v>-3.9430000000000001</v>
       </c>
       <c r="O50" s="1">
-        <v>-6.4</v>
+        <v>4.54</v>
       </c>
       <c r="P50" s="1">
-        <v>4.2</v>
+        <v>0.95699999999999985</v>
       </c>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
@@ -4548,27 +4550,29 @@
         <v>32</v>
       </c>
       <c r="T50" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U50" s="1">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="V50" s="1">
-        <v>-36.32</v>
+        <v>4.2</v>
       </c>
       <c r="W50" s="1">
-        <v>-2.8079999999999998</v>
+        <v>-0.34200000000000003</v>
       </c>
       <c r="X50" s="1">
-        <v>0</v>
+        <v>16.8</v>
       </c>
       <c r="Y50" s="1">
-        <v>1.9950000000000001</v>
+        <v>8.4</v>
       </c>
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
       <c r="AB50" s="1"/>
-      <c r="AC50" s="1"/>
+      <c r="AC50" s="2" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
@@ -4576,13 +4580,13 @@
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D51" s="1">
         <v>4.54</v>
       </c>
       <c r="E51" s="1">
-        <v>-2.9860000000000002</v>
+        <v>-6.1</v>
       </c>
       <c r="F51" s="1">
         <v>8.6199999999999992</v>
@@ -4597,23 +4601,23 @@
         <v>8.85</v>
       </c>
       <c r="J51" s="1">
-        <v>-2.6</v>
+        <v>-5.6999999999999993</v>
       </c>
       <c r="K51" s="1">
-        <v>-3.4</v>
+        <v>-6.5</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1">
         <v>0</v>
       </c>
       <c r="N51" s="1">
-        <v>-3.9430000000000001</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="O51" s="1">
         <v>4.54</v>
       </c>
       <c r="P51" s="1">
-        <v>0.95699999999999985</v>
+        <v>-10.016</v>
       </c>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
@@ -4627,7 +4631,7 @@
         <v>8</v>
       </c>
       <c r="V51" s="1">
-        <v>4.2</v>
+        <v>-4.2</v>
       </c>
       <c r="W51" s="1">
         <v>-0.34200000000000003</v>
@@ -4642,7 +4646,7 @@
       <c r="AA51" s="1"/>
       <c r="AB51" s="1"/>
       <c r="AC51" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.45">
@@ -4651,44 +4655,44 @@
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D52" s="1">
-        <v>4.54</v>
+        <v>-6.62</v>
       </c>
       <c r="E52" s="1">
-        <v>-6.1</v>
+        <v>1.4750000000000001</v>
       </c>
       <c r="F52" s="1">
-        <v>8.6199999999999992</v>
+        <v>1.44</v>
       </c>
       <c r="G52" s="1">
-        <v>0.8</v>
+        <v>2.95</v>
       </c>
       <c r="H52" s="1">
-        <v>0.2300000000000004</v>
+        <v>-7.34</v>
       </c>
       <c r="I52" s="1">
-        <v>8.85</v>
+        <v>-5.9</v>
       </c>
       <c r="J52" s="1">
-        <v>-5.6999999999999993</v>
+        <v>2.95</v>
       </c>
       <c r="K52" s="1">
-        <v>-6.5</v>
+        <v>0</v>
       </c>
       <c r="L52" s="1"/>
       <c r="M52" s="1">
         <v>0</v>
       </c>
       <c r="N52" s="1">
-        <v>3.9159999999999999</v>
+        <v>0</v>
       </c>
       <c r="O52" s="1">
-        <v>4.54</v>
+        <v>-6.62</v>
       </c>
       <c r="P52" s="1">
-        <v>-10.016</v>
+        <v>1.4750000000000001</v>
       </c>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
@@ -4696,29 +4700,27 @@
         <v>32</v>
       </c>
       <c r="T52" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U52" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="V52" s="1">
-        <v>-4.2</v>
+        <v>0</v>
       </c>
       <c r="W52" s="1">
-        <v>-0.34200000000000003</v>
+        <v>-18.378</v>
       </c>
       <c r="X52" s="1">
-        <v>16.8</v>
+        <v>71</v>
       </c>
       <c r="Y52" s="1">
-        <v>8.4</v>
+        <v>0</v>
       </c>
       <c r="Z52" s="1"/>
       <c r="AA52" s="1"/>
       <c r="AB52" s="1"/>
-      <c r="AC52" s="2" t="s">
-        <v>279</v>
-      </c>
+      <c r="AC52" s="1"/>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
@@ -4726,28 +4728,28 @@
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D53" s="1">
-        <v>-6.62</v>
+        <v>6.9</v>
       </c>
       <c r="E53" s="1">
-        <v>1.4750000000000001</v>
+        <v>3.9</v>
       </c>
       <c r="F53" s="1">
-        <v>1.44</v>
+        <v>7.8</v>
       </c>
       <c r="G53" s="1">
-        <v>2.95</v>
+        <v>7.8</v>
       </c>
       <c r="H53" s="1">
-        <v>-7.34</v>
+        <v>3</v>
       </c>
       <c r="I53" s="1">
-        <v>-5.9</v>
+        <v>10.8</v>
       </c>
       <c r="J53" s="1">
-        <v>2.95</v>
+        <v>7.8</v>
       </c>
       <c r="K53" s="1">
         <v>0</v>
@@ -4760,10 +4762,10 @@
         <v>0</v>
       </c>
       <c r="O53" s="1">
-        <v>-6.62</v>
+        <v>6.9</v>
       </c>
       <c r="P53" s="1">
-        <v>1.4750000000000001</v>
+        <v>3.9</v>
       </c>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
@@ -4771,27 +4773,29 @@
         <v>32</v>
       </c>
       <c r="T53" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="U53" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="V53" s="1">
         <v>0</v>
       </c>
       <c r="W53" s="1">
-        <v>-18.378</v>
+        <v>-0.34200000000000003</v>
       </c>
       <c r="X53" s="1">
-        <v>71</v>
+        <v>8.4</v>
       </c>
       <c r="Y53" s="1">
-        <v>0</v>
+        <v>8.4</v>
       </c>
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
       <c r="AB53" s="1"/>
-      <c r="AC53" s="1"/>
+      <c r="AC53" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
@@ -4799,31 +4803,31 @@
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D54" s="1">
-        <v>6.9</v>
+        <v>-4.8579999999999997</v>
       </c>
       <c r="E54" s="1">
-        <v>3.9</v>
+        <v>-0.76100000000000001</v>
       </c>
       <c r="F54" s="1">
-        <v>7.8</v>
+        <v>1.012</v>
       </c>
       <c r="G54" s="1">
-        <v>7.8</v>
+        <v>1.089</v>
       </c>
       <c r="H54" s="1">
-        <v>3</v>
+        <v>-5.3639999999999999</v>
       </c>
       <c r="I54" s="1">
-        <v>10.8</v>
+        <v>-4.3519999999999994</v>
       </c>
       <c r="J54" s="1">
-        <v>7.8</v>
+        <v>-0.217</v>
       </c>
       <c r="K54" s="1">
-        <v>0</v>
+        <v>-1.306</v>
       </c>
       <c r="L54" s="1"/>
       <c r="M54" s="1">
@@ -4833,10 +4837,10 @@
         <v>0</v>
       </c>
       <c r="O54" s="1">
-        <v>6.9</v>
+        <v>-4.8579999999999997</v>
       </c>
       <c r="P54" s="1">
-        <v>3.9</v>
+        <v>-0.76100000000000001</v>
       </c>
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
@@ -4844,61 +4848,59 @@
         <v>32</v>
       </c>
       <c r="T54" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="U54" s="1">
         <v>8</v>
       </c>
       <c r="V54" s="1">
-        <v>0</v>
+        <v>-34.658999999999999</v>
       </c>
       <c r="W54" s="1">
-        <v>-0.34200000000000003</v>
+        <v>-0.13500000000000001</v>
       </c>
       <c r="X54" s="1">
-        <v>8.4</v>
+        <v>0</v>
       </c>
       <c r="Y54" s="1">
-        <v>8.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
       <c r="AB54" s="1"/>
-      <c r="AC54" s="2" t="s">
-        <v>283</v>
-      </c>
+      <c r="AC54" s="1"/>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D55" s="1">
-        <v>-4.8579999999999997</v>
+        <v>-7.89</v>
       </c>
       <c r="E55" s="1">
-        <v>-0.76100000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="F55" s="1">
-        <v>1.012</v>
+        <v>1</v>
       </c>
       <c r="G55" s="1">
-        <v>1.089</v>
+        <v>10.4</v>
       </c>
       <c r="H55" s="1">
-        <v>-5.3639999999999999</v>
+        <v>-8.39</v>
       </c>
       <c r="I55" s="1">
-        <v>-4.3519999999999994</v>
+        <v>-7.39</v>
       </c>
       <c r="J55" s="1">
-        <v>-0.217</v>
+        <v>10.4</v>
       </c>
       <c r="K55" s="1">
-        <v>-1.306</v>
+        <v>0</v>
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1">
@@ -4908,10 +4910,10 @@
         <v>0</v>
       </c>
       <c r="O55" s="1">
-        <v>-4.8579999999999997</v>
+        <v>-7.89</v>
       </c>
       <c r="P55" s="1">
-        <v>-0.76100000000000001</v>
+        <v>5.2</v>
       </c>
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
@@ -4919,22 +4921,22 @@
         <v>32</v>
       </c>
       <c r="T55" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U55" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V55" s="1">
-        <v>-34.658999999999999</v>
+        <v>-1E-3</v>
       </c>
       <c r="W55" s="1">
-        <v>-0.13500000000000001</v>
+        <v>2.2170000000000001</v>
       </c>
       <c r="X55" s="1">
-        <v>0</v>
+        <v>72.8</v>
       </c>
       <c r="Y55" s="1">
-        <v>8.1999999999999993</v>
+        <v>10</v>
       </c>
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
@@ -4943,48 +4945,48 @@
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D56" s="1">
-        <v>-7.89</v>
+        <v>-2.25</v>
       </c>
       <c r="E56" s="1">
-        <v>5.2</v>
+        <v>-4.7</v>
       </c>
       <c r="F56" s="1">
-        <v>1</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G56" s="1">
-        <v>10.4</v>
+        <v>0.6</v>
       </c>
       <c r="H56" s="1">
-        <v>-8.39</v>
+        <v>-4.45</v>
       </c>
       <c r="I56" s="1">
-        <v>-7.39</v>
+        <v>-4.9999999999999822E-2</v>
       </c>
       <c r="J56" s="1">
-        <v>10.4</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="K56" s="1">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1">
         <v>0</v>
       </c>
       <c r="N56" s="1">
-        <v>0</v>
+        <v>-3.9159999999999999</v>
       </c>
       <c r="O56" s="1">
-        <v>-7.89</v>
+        <v>-2.25</v>
       </c>
       <c r="P56" s="1">
-        <v>5.2</v>
+        <v>-0.78400000000000025</v>
       </c>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
@@ -4992,27 +4994,29 @@
         <v>32</v>
       </c>
       <c r="T56" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U56" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="V56" s="1">
-        <v>-1E-3</v>
+        <v>4.2</v>
       </c>
       <c r="W56" s="1">
-        <v>2.2170000000000001</v>
+        <v>-0.34200000000000003</v>
       </c>
       <c r="X56" s="1">
-        <v>72.8</v>
+        <v>16.8</v>
       </c>
       <c r="Y56" s="1">
-        <v>10</v>
+        <v>8.4</v>
       </c>
       <c r="Z56" s="1"/>
       <c r="AA56" s="1"/>
       <c r="AB56" s="1"/>
-      <c r="AC56" s="1"/>
+      <c r="AC56" s="2" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
@@ -5020,10 +5024,10 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D57" s="1">
-        <v>-2.25</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E57" s="1">
         <v>-4.7</v>
@@ -5035,10 +5039,10 @@
         <v>0.6</v>
       </c>
       <c r="H57" s="1">
-        <v>-4.45</v>
+        <v>0</v>
       </c>
       <c r="I57" s="1">
-        <v>-4.9999999999999822E-2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J57" s="1">
         <v>-4.4000000000000004</v>
@@ -5051,13 +5055,13 @@
         <v>0</v>
       </c>
       <c r="N57" s="1">
-        <v>-3.9159999999999999</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="O57" s="1">
-        <v>-2.25</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="P57" s="1">
-        <v>-0.78400000000000025</v>
+        <v>-8.6159999999999997</v>
       </c>
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
@@ -5071,7 +5075,7 @@
         <v>8</v>
       </c>
       <c r="V57" s="1">
-        <v>4.2</v>
+        <v>-4.2</v>
       </c>
       <c r="W57" s="1">
         <v>-0.34200000000000003</v>
@@ -5086,53 +5090,53 @@
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
       <c r="AC57" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D58" s="1">
-        <v>2.2000000000000002</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="E58" s="1">
-        <v>-4.7</v>
+        <v>-10.5</v>
       </c>
       <c r="F58" s="1">
-        <v>4.4000000000000004</v>
+        <v>15.4</v>
       </c>
       <c r="G58" s="1">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="H58" s="1">
-        <v>0</v>
+        <v>-5.25</v>
       </c>
       <c r="I58" s="1">
-        <v>4.4000000000000004</v>
+        <v>10.15</v>
       </c>
       <c r="J58" s="1">
-        <v>-4.4000000000000004</v>
+        <v>-10.3</v>
       </c>
       <c r="K58" s="1">
-        <v>-5</v>
+        <v>-10.7</v>
       </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1">
         <v>0</v>
       </c>
       <c r="N58" s="1">
-        <v>3.9159999999999999</v>
+        <v>0</v>
       </c>
       <c r="O58" s="1">
-        <v>2.2000000000000002</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="P58" s="1">
-        <v>-8.6159999999999997</v>
+        <v>-10.5</v>
       </c>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
@@ -5140,29 +5144,27 @@
         <v>32</v>
       </c>
       <c r="T58" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U58" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V58" s="1">
-        <v>-4.2</v>
+        <v>-0.5</v>
       </c>
       <c r="W58" s="1">
-        <v>-0.34200000000000003</v>
+        <v>0</v>
       </c>
       <c r="X58" s="1">
-        <v>16.8</v>
+        <v>15</v>
       </c>
       <c r="Y58" s="1">
-        <v>8.4</v>
+        <v>72.680000000000007</v>
       </c>
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
-      <c r="AC58" s="2" t="s">
-        <v>279</v>
-      </c>
+      <c r="AC58" s="1"/>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
@@ -5170,31 +5172,31 @@
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D59" s="1">
-        <v>2.4500000000000002</v>
+        <v>-10.59</v>
       </c>
       <c r="E59" s="1">
-        <v>-10.5</v>
+        <v>-3.0750000000000002</v>
       </c>
       <c r="F59" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="G59" s="1">
         <v>15.4</v>
       </c>
-      <c r="G59" s="1">
-        <v>0.4</v>
-      </c>
       <c r="H59" s="1">
-        <v>-5.25</v>
+        <v>-10.79</v>
       </c>
       <c r="I59" s="1">
-        <v>10.15</v>
+        <v>-10.39</v>
       </c>
       <c r="J59" s="1">
-        <v>-10.3</v>
+        <v>4.625</v>
       </c>
       <c r="K59" s="1">
-        <v>-10.7</v>
+        <v>-10.775</v>
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1">
@@ -5204,10 +5206,10 @@
         <v>0</v>
       </c>
       <c r="O59" s="1">
-        <v>2.4500000000000002</v>
+        <v>-10.59</v>
       </c>
       <c r="P59" s="1">
-        <v>-10.5</v>
+        <v>-3.0750000000000002</v>
       </c>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
@@ -5215,22 +5217,22 @@
         <v>32</v>
       </c>
       <c r="T59" s="1">
+        <v>2</v>
+      </c>
+      <c r="U59" s="1">
         <v>6</v>
       </c>
-      <c r="U59" s="1">
-        <v>2</v>
-      </c>
       <c r="V59" s="1">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="W59" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X59" s="1">
+        <v>74</v>
+      </c>
+      <c r="Y59" s="1">
         <v>15</v>
-      </c>
-      <c r="Y59" s="1">
-        <v>72.680000000000007</v>
       </c>
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
@@ -5239,48 +5241,48 @@
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>66</v>
+        <v>198</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>68</v>
+        <v>199</v>
       </c>
       <c r="D60" s="1">
-        <v>-10.59</v>
+        <v>-3.15</v>
       </c>
       <c r="E60" s="1">
-        <v>-3.0750000000000002</v>
+        <v>-0.96</v>
       </c>
       <c r="F60" s="1">
-        <v>0.4</v>
+        <v>1.6339999999999999</v>
       </c>
       <c r="G60" s="1">
-        <v>15.4</v>
+        <v>0.62</v>
       </c>
       <c r="H60" s="1">
-        <v>-10.79</v>
+        <v>-3.9670000000000001</v>
       </c>
       <c r="I60" s="1">
-        <v>-10.39</v>
+        <v>-2.3330000000000002</v>
       </c>
       <c r="J60" s="1">
-        <v>4.625</v>
+        <v>-0.64999999999999991</v>
       </c>
       <c r="K60" s="1">
-        <v>-10.775</v>
+        <v>-1.27</v>
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1">
-        <v>0</v>
+        <v>-1.629</v>
       </c>
       <c r="N60" s="1">
-        <v>0</v>
+        <v>-3.9159999999999999</v>
       </c>
       <c r="O60" s="1">
-        <v>-10.59</v>
+        <v>-1.5209999999999999</v>
       </c>
       <c r="P60" s="1">
-        <v>-3.0750000000000002</v>
+        <v>2.956</v>
       </c>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -5288,22 +5290,22 @@
         <v>32</v>
       </c>
       <c r="T60" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U60" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="V60" s="1">
-        <v>0</v>
+        <v>-29.4</v>
       </c>
       <c r="W60" s="1">
-        <v>-1</v>
+        <v>-4.5419999999999998</v>
       </c>
       <c r="X60" s="1">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="Y60" s="1">
-        <v>15</v>
+        <v>16.8</v>
       </c>
       <c r="Z60" s="1"/>
       <c r="AA60" s="1"/>
@@ -5316,13 +5318,13 @@
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D61" s="1">
         <v>-3.15</v>
       </c>
       <c r="E61" s="1">
-        <v>-0.96</v>
+        <v>-1.63</v>
       </c>
       <c r="F61" s="1">
         <v>1.6339999999999999</v>
@@ -5337,23 +5339,23 @@
         <v>-2.3330000000000002</v>
       </c>
       <c r="J61" s="1">
-        <v>-0.64999999999999991</v>
+        <v>-1.32</v>
       </c>
       <c r="K61" s="1">
-        <v>-1.27</v>
+        <v>-1.94</v>
       </c>
       <c r="L61" s="1"/>
       <c r="M61" s="1">
-        <v>-1.629</v>
+        <v>1.629</v>
       </c>
       <c r="N61" s="1">
-        <v>-3.9159999999999999</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="O61" s="1">
-        <v>-1.5209999999999999</v>
+        <v>-4.7789999999999999</v>
       </c>
       <c r="P61" s="1">
-        <v>2.956</v>
+        <v>-5.5459999999999994</v>
       </c>
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
@@ -5367,7 +5369,7 @@
         <v>3</v>
       </c>
       <c r="V61" s="1">
-        <v>-29.4</v>
+        <v>29.4</v>
       </c>
       <c r="W61" s="1">
         <v>-4.5419999999999998</v>
@@ -5417,16 +5419,16 @@
       </c>
       <c r="L62" s="1"/>
       <c r="M62" s="1">
-        <v>1.629</v>
+        <v>0</v>
       </c>
       <c r="N62" s="1">
-        <v>3.9159999999999999</v>
+        <v>0</v>
       </c>
       <c r="O62" s="1">
-        <v>-4.7789999999999999</v>
+        <v>-3.15</v>
       </c>
       <c r="P62" s="1">
-        <v>-5.5459999999999994</v>
+        <v>-1.63</v>
       </c>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
@@ -5437,19 +5439,19 @@
         <v>1</v>
       </c>
       <c r="U62" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V62" s="1">
-        <v>29.4</v>
+        <v>22.629000000000001</v>
       </c>
       <c r="W62" s="1">
-        <v>-4.5419999999999998</v>
+        <v>-33.658000000000001</v>
       </c>
       <c r="X62" s="1">
         <v>0</v>
       </c>
       <c r="Y62" s="1">
-        <v>16.8</v>
+        <v>0</v>
       </c>
       <c r="Z62" s="1"/>
       <c r="AA62" s="1"/>
@@ -5462,44 +5464,44 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D63" s="1">
-        <v>-3.15</v>
+        <v>1.3540000000000001</v>
       </c>
       <c r="E63" s="1">
-        <v>-1.63</v>
+        <v>-5.36</v>
       </c>
       <c r="F63" s="1">
-        <v>1.6339999999999999</v>
+        <v>4.8920000000000003</v>
       </c>
       <c r="G63" s="1">
         <v>0.62</v>
       </c>
       <c r="H63" s="1">
-        <v>-3.9670000000000001</v>
+        <v>-1.0920000000000001</v>
       </c>
       <c r="I63" s="1">
-        <v>-2.3330000000000002</v>
+        <v>3.8</v>
       </c>
       <c r="J63" s="1">
-        <v>-1.32</v>
+        <v>-5.0500000000000007</v>
       </c>
       <c r="K63" s="1">
-        <v>-1.94</v>
+        <v>-5.67</v>
       </c>
       <c r="L63" s="1"/>
       <c r="M63" s="1">
         <v>0</v>
       </c>
       <c r="N63" s="1">
-        <v>0</v>
+        <v>-3.9159999999999999</v>
       </c>
       <c r="O63" s="1">
-        <v>-3.15</v>
+        <v>1.3540000000000001</v>
       </c>
       <c r="P63" s="1">
-        <v>-1.63</v>
+        <v>-1.444</v>
       </c>
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
@@ -5507,27 +5509,29 @@
         <v>32</v>
       </c>
       <c r="T63" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U63" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="V63" s="1">
-        <v>22.629000000000001</v>
+        <v>4.2</v>
       </c>
       <c r="W63" s="1">
-        <v>-33.658000000000001</v>
+        <v>-0.34200000000000003</v>
       </c>
       <c r="X63" s="1">
-        <v>0</v>
+        <v>16.8</v>
       </c>
       <c r="Y63" s="1">
-        <v>0</v>
+        <v>8.4</v>
       </c>
       <c r="Z63" s="1"/>
       <c r="AA63" s="1"/>
       <c r="AB63" s="1"/>
-      <c r="AC63" s="1"/>
+      <c r="AC63" s="2" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
@@ -5566,13 +5570,13 @@
         <v>0</v>
       </c>
       <c r="N64" s="1">
-        <v>-3.9159999999999999</v>
+        <v>3.9159999999999999</v>
       </c>
       <c r="O64" s="1">
         <v>1.3540000000000001</v>
       </c>
       <c r="P64" s="1">
-        <v>-1.444</v>
+        <v>-9.2759999999999998</v>
       </c>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
@@ -5586,7 +5590,7 @@
         <v>8</v>
       </c>
       <c r="V64" s="1">
-        <v>4.2</v>
+        <v>-4.2</v>
       </c>
       <c r="W64" s="1">
         <v>-0.34200000000000003</v>
@@ -5601,157 +5605,154 @@
       <c r="AA64" s="1"/>
       <c r="AB64" s="1"/>
       <c r="AC64" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A65" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D65" s="1">
-        <v>1.3540000000000001</v>
-      </c>
-      <c r="E65" s="1">
-        <v>-5.36</v>
-      </c>
-      <c r="F65" s="1">
-        <v>4.8920000000000003</v>
-      </c>
-      <c r="G65" s="1">
-        <v>0.62</v>
-      </c>
-      <c r="H65" s="1">
-        <v>-1.0920000000000001</v>
-      </c>
-      <c r="I65" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="J65" s="1">
-        <v>-5.0500000000000007</v>
-      </c>
-      <c r="K65" s="1">
-        <v>-5.67</v>
-      </c>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1">
-        <v>0</v>
-      </c>
-      <c r="N65" s="1">
-        <v>3.9159999999999999</v>
-      </c>
-      <c r="O65" s="1">
-        <v>1.3540000000000001</v>
-      </c>
-      <c r="P65" s="1">
-        <v>-9.2759999999999998</v>
-      </c>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-      <c r="S65" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="65" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D65" s="5">
+        <v>-6.45</v>
+      </c>
+      <c r="E65" s="5">
+        <v>7</v>
+      </c>
+      <c r="F65" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G65" s="5">
+        <v>3.1</v>
+      </c>
+      <c r="H65" s="5">
+        <v>-7</v>
+      </c>
+      <c r="I65" s="5">
+        <v>-5.9</v>
+      </c>
+      <c r="J65" s="5">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="K65" s="5">
+        <v>5.45</v>
+      </c>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5">
+        <v>0</v>
+      </c>
+      <c r="N65" s="5">
+        <v>-1.2999999999999999E-2</v>
+      </c>
+      <c r="O65" s="5">
+        <v>-6.45</v>
+      </c>
+      <c r="P65" s="5">
+        <v>7.0129999999999999</v>
+      </c>
+      <c r="Q65" s="5"/>
+      <c r="R65" s="5"/>
+      <c r="S65" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T65" s="1">
+      <c r="T65" s="5">
+        <v>9</v>
+      </c>
+      <c r="U65" s="5">
+        <v>16</v>
+      </c>
+      <c r="V65" s="5">
+        <v>0</v>
+      </c>
+      <c r="W65" s="5">
+        <v>-0.32800000000000001</v>
+      </c>
+      <c r="X65" s="5">
+        <v>8.4</v>
+      </c>
+      <c r="Y65" s="5">
         <v>4</v>
       </c>
-      <c r="U65" s="1">
-        <v>8</v>
-      </c>
-      <c r="V65" s="1">
-        <v>-4.2</v>
-      </c>
-      <c r="W65" s="1">
-        <v>-0.34200000000000003</v>
-      </c>
-      <c r="X65" s="1">
-        <v>16.8</v>
-      </c>
-      <c r="Y65" s="1">
-        <v>8.4</v>
-      </c>
-      <c r="Z65" s="1"/>
-      <c r="AA65" s="1"/>
-      <c r="AB65" s="1"/>
-      <c r="AC65" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="66" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D66" s="5">
-        <v>-6.45</v>
-      </c>
-      <c r="E66" s="5">
-        <v>7</v>
-      </c>
-      <c r="F66" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G66" s="5">
-        <v>3.1</v>
-      </c>
-      <c r="H66" s="5">
-        <v>-7</v>
-      </c>
-      <c r="I66" s="5">
-        <v>-5.9</v>
-      </c>
-      <c r="J66" s="5">
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="K66" s="5">
-        <v>5.45</v>
-      </c>
-      <c r="L66" s="5"/>
-      <c r="M66" s="5">
-        <v>0</v>
-      </c>
-      <c r="N66" s="5">
-        <v>-1.2999999999999999E-2</v>
-      </c>
-      <c r="O66" s="5">
-        <v>-6.45</v>
-      </c>
-      <c r="P66" s="5">
-        <v>7.0129999999999999</v>
-      </c>
-      <c r="Q66" s="5"/>
-      <c r="R66" s="5"/>
-      <c r="S66" s="5" t="s">
+      <c r="Z65" s="5"/>
+      <c r="AA65" s="5"/>
+      <c r="AB65" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D66" s="34">
+        <v>-1.8</v>
+      </c>
+      <c r="E66" s="34">
+        <v>-9.625</v>
+      </c>
+      <c r="F66" s="34">
+        <v>6.6</v>
+      </c>
+      <c r="G66" s="34">
+        <v>1.3</v>
+      </c>
+      <c r="H66" s="34">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="I66" s="34">
+        <v>1.5</v>
+      </c>
+      <c r="J66" s="34">
+        <v>-8.9749999999999996</v>
+      </c>
+      <c r="K66" s="34">
+        <v>-10.275</v>
+      </c>
+      <c r="L66" s="34"/>
+      <c r="M66" s="34">
+        <v>0</v>
+      </c>
+      <c r="N66" s="34">
+        <v>0</v>
+      </c>
+      <c r="O66" s="34">
+        <v>-1.8</v>
+      </c>
+      <c r="P66" s="34">
+        <v>-9.625</v>
+      </c>
+      <c r="Q66" s="34"/>
+      <c r="R66" s="34"/>
+      <c r="S66" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T66" s="5">
-        <v>9</v>
-      </c>
-      <c r="U66" s="5">
-        <v>16</v>
-      </c>
-      <c r="V66" s="5">
-        <v>0</v>
-      </c>
-      <c r="W66" s="5">
-        <v>-0.32800000000000001</v>
-      </c>
-      <c r="X66" s="5">
-        <v>8.4</v>
-      </c>
-      <c r="Y66" s="5">
+      <c r="T66" s="34">
         <v>4</v>
       </c>
-      <c r="Z66" s="5"/>
-      <c r="AA66" s="5"/>
-      <c r="AB66" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="U66" s="34">
+        <v>2</v>
+      </c>
+      <c r="V66" s="34">
+        <v>-3.85</v>
+      </c>
+      <c r="W66" s="34">
+        <v>0</v>
+      </c>
+      <c r="X66" s="34">
+        <v>6.4</v>
+      </c>
+      <c r="Y66" s="34">
+        <v>71.290000000000006</v>
+      </c>
+      <c r="Z66" s="34"/>
+      <c r="AA66" s="34"/>
+      <c r="AB66" s="34"/>
     </row>
     <row r="67" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A67" s="5" t="s">
@@ -5973,77 +5974,77 @@
       <c r="AB69" s="1"/>
       <c r="AC69" s="1"/>
     </row>
-    <row r="70" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A70" s="27" t="s">
+    <row r="70" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A70" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="B70" s="27"/>
-      <c r="C70" s="27" t="s">
+      <c r="B70" s="34"/>
+      <c r="C70" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="D70" s="27">
+      <c r="D70" s="34">
         <v>-5.4</v>
       </c>
-      <c r="E70" s="27">
+      <c r="E70" s="34">
         <v>-8.375</v>
       </c>
-      <c r="F70" s="27">
+      <c r="F70" s="34">
         <v>0.5</v>
       </c>
-      <c r="G70" s="27">
+      <c r="G70" s="34">
         <v>0.8</v>
       </c>
-      <c r="H70" s="27">
+      <c r="H70" s="34">
         <v>-5.65</v>
       </c>
-      <c r="I70" s="27">
+      <c r="I70" s="34">
         <v>-5.15</v>
       </c>
-      <c r="J70" s="27">
+      <c r="J70" s="34">
         <v>-7.9749999999999996</v>
       </c>
-      <c r="K70" s="27">
+      <c r="K70" s="34">
         <v>-8.7750000000000004</v>
       </c>
-      <c r="L70" s="27"/>
-      <c r="M70" s="27">
-        <v>0</v>
-      </c>
-      <c r="N70" s="27">
-        <v>0</v>
-      </c>
-      <c r="O70" s="27">
+      <c r="L70" s="34"/>
+      <c r="M70" s="34">
+        <v>0</v>
+      </c>
+      <c r="N70" s="34">
+        <v>0</v>
+      </c>
+      <c r="O70" s="34">
         <v>-5.4</v>
       </c>
-      <c r="P70" s="27">
+      <c r="P70" s="34">
         <v>-8.375</v>
       </c>
-      <c r="Q70" s="27"/>
-      <c r="R70" s="27"/>
-      <c r="S70" s="27" t="s">
+      <c r="Q70" s="34"/>
+      <c r="R70" s="34"/>
+      <c r="S70" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T70" s="27">
+      <c r="T70" s="34">
         <v>2</v>
       </c>
-      <c r="U70" s="27">
-        <v>1</v>
-      </c>
-      <c r="V70" s="27">
+      <c r="U70" s="34">
+        <v>1</v>
+      </c>
+      <c r="V70" s="34">
         <v>-3.85</v>
       </c>
-      <c r="W70" s="27">
+      <c r="W70" s="34">
         <v>34.015000000000001</v>
       </c>
-      <c r="X70" s="27">
+      <c r="X70" s="34">
         <v>45.7</v>
       </c>
-      <c r="Y70" s="27">
+      <c r="Y70" s="34">
         <v>0.32500000000000001</v>
       </c>
-      <c r="Z70" s="27"/>
-      <c r="AA70" s="27"/>
-      <c r="AB70" s="27"/>
+      <c r="Z70" s="34"/>
+      <c r="AA70" s="34"/>
+      <c r="AB70" s="34"/>
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
@@ -6414,77 +6415,77 @@
         <v>279</v>
       </c>
     </row>
-    <row r="76" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="27" t="s">
+    <row r="76" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A76" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B76" s="27"/>
-      <c r="C76" s="27" t="s">
+      <c r="B76" s="34"/>
+      <c r="C76" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="D76" s="27">
+      <c r="D76" s="34">
         <v>-6.39</v>
       </c>
-      <c r="E76" s="27">
+      <c r="E76" s="34">
         <v>10.5</v>
       </c>
-      <c r="F76" s="27">
+      <c r="F76" s="34">
         <v>1.9</v>
       </c>
-      <c r="G76" s="27">
+      <c r="G76" s="34">
         <v>2.4</v>
       </c>
-      <c r="H76" s="27">
+      <c r="H76" s="34">
         <v>-7.34</v>
       </c>
-      <c r="I76" s="27">
+      <c r="I76" s="34">
         <v>-5.44</v>
       </c>
-      <c r="J76" s="27">
+      <c r="J76" s="34">
         <v>11.7</v>
       </c>
-      <c r="K76" s="27">
+      <c r="K76" s="34">
         <v>9.3000000000000007</v>
       </c>
-      <c r="L76" s="27"/>
-      <c r="M76" s="27">
-        <v>0</v>
-      </c>
-      <c r="N76" s="27">
-        <v>0</v>
-      </c>
-      <c r="O76" s="27">
+      <c r="L76" s="34"/>
+      <c r="M76" s="34">
+        <v>0</v>
+      </c>
+      <c r="N76" s="34">
+        <v>0</v>
+      </c>
+      <c r="O76" s="34">
         <v>-6.39</v>
       </c>
-      <c r="P76" s="27">
+      <c r="P76" s="34">
         <v>10.5</v>
       </c>
-      <c r="Q76" s="27"/>
-      <c r="R76" s="27"/>
-      <c r="S76" s="27" t="s">
+      <c r="Q76" s="34"/>
+      <c r="R76" s="34"/>
+      <c r="S76" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T76" s="27">
+      <c r="T76" s="34">
         <v>2</v>
       </c>
-      <c r="U76" s="27">
-        <v>1</v>
-      </c>
-      <c r="V76" s="27">
+      <c r="U76" s="34">
+        <v>1</v>
+      </c>
+      <c r="V76" s="34">
         <v>-3.85</v>
       </c>
-      <c r="W76" s="27">
+      <c r="W76" s="34">
         <v>35.179000000000002</v>
       </c>
-      <c r="X76" s="27">
+      <c r="X76" s="34">
         <v>45.7</v>
       </c>
-      <c r="Y76" s="27">
+      <c r="Y76" s="34">
         <v>3.8119999999999998</v>
       </c>
-      <c r="Z76" s="27"/>
-      <c r="AA76" s="27"/>
-      <c r="AB76" s="27"/>
+      <c r="Z76" s="34"/>
+      <c r="AA76" s="34"/>
+      <c r="AB76" s="34"/>
     </row>
     <row r="77" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
@@ -7952,221 +7953,221 @@
       <c r="AB96" s="1"/>
       <c r="AC96" s="1"/>
     </row>
-    <row r="97" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="27" t="s">
+    <row r="97" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A97" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B97" s="27"/>
-      <c r="C97" s="27" t="s">
+      <c r="B97" s="34"/>
+      <c r="C97" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="D97" s="27">
+      <c r="D97" s="34">
         <v>-3.0489999999999999</v>
       </c>
-      <c r="E97" s="27">
+      <c r="E97" s="34">
         <v>9.5500000000000007</v>
       </c>
-      <c r="F97" s="27">
+      <c r="F97" s="34">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G97" s="27">
+      <c r="G97" s="34">
         <v>0.5</v>
       </c>
-      <c r="H97" s="27">
+      <c r="H97" s="34">
         <v>-5.3490000000000002</v>
       </c>
-      <c r="I97" s="27">
+      <c r="I97" s="34">
         <v>-0.74900000000000011</v>
       </c>
-      <c r="J97" s="27">
+      <c r="J97" s="34">
         <v>9.8000000000000007</v>
       </c>
-      <c r="K97" s="27">
+      <c r="K97" s="34">
         <v>9.3000000000000007</v>
       </c>
-      <c r="L97" s="27"/>
-      <c r="M97" s="27">
-        <v>0</v>
-      </c>
-      <c r="N97" s="27">
-        <v>0</v>
-      </c>
-      <c r="O97" s="27">
+      <c r="L97" s="34"/>
+      <c r="M97" s="34">
+        <v>0</v>
+      </c>
+      <c r="N97" s="34">
+        <v>0</v>
+      </c>
+      <c r="O97" s="34">
         <v>-3.0489999999999999</v>
       </c>
-      <c r="P97" s="27">
+      <c r="P97" s="34">
         <v>9.5500000000000007</v>
       </c>
-      <c r="Q97" s="27"/>
-      <c r="R97" s="27"/>
-      <c r="S97" s="27" t="s">
+      <c r="Q97" s="34"/>
+      <c r="R97" s="34"/>
+      <c r="S97" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T97" s="27">
+      <c r="T97" s="34">
         <v>2</v>
       </c>
-      <c r="U97" s="27">
-        <v>1</v>
-      </c>
-      <c r="V97" s="27">
+      <c r="U97" s="34">
+        <v>1</v>
+      </c>
+      <c r="V97" s="34">
         <v>30</v>
       </c>
-      <c r="W97" s="27">
+      <c r="W97" s="34">
         <v>24.957999999999998</v>
       </c>
-      <c r="X97" s="27">
+      <c r="X97" s="34">
         <v>4.0999999999999996</v>
       </c>
-      <c r="Y97" s="27">
-        <v>0</v>
-      </c>
-      <c r="Z97" s="27"/>
-      <c r="AA97" s="27"/>
-      <c r="AB97" s="27"/>
-    </row>
-    <row r="98" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="27" t="s">
+      <c r="Y97" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z97" s="34"/>
+      <c r="AA97" s="34"/>
+      <c r="AB97" s="34"/>
+    </row>
+    <row r="98" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A98" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B98" s="27"/>
-      <c r="C98" s="27" t="s">
+      <c r="B98" s="34"/>
+      <c r="C98" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="D98" s="27">
+      <c r="D98" s="34">
         <v>-3.0489999999999999</v>
       </c>
-      <c r="E98" s="27">
+      <c r="E98" s="34">
         <v>9.5500000000000007</v>
       </c>
-      <c r="F98" s="27">
+      <c r="F98" s="34">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G98" s="27">
+      <c r="G98" s="34">
         <v>0.5</v>
       </c>
-      <c r="H98" s="27">
+      <c r="H98" s="34">
         <v>-5.3490000000000002</v>
       </c>
-      <c r="I98" s="27">
+      <c r="I98" s="34">
         <v>-0.74900000000000011</v>
       </c>
-      <c r="J98" s="27">
+      <c r="J98" s="34">
         <v>9.8000000000000007</v>
       </c>
-      <c r="K98" s="27">
+      <c r="K98" s="34">
         <v>9.3000000000000007</v>
       </c>
-      <c r="L98" s="27"/>
-      <c r="M98" s="27">
-        <v>0</v>
-      </c>
-      <c r="N98" s="27">
-        <v>0</v>
-      </c>
-      <c r="O98" s="27">
+      <c r="L98" s="34"/>
+      <c r="M98" s="34">
+        <v>0</v>
+      </c>
+      <c r="N98" s="34">
+        <v>0</v>
+      </c>
+      <c r="O98" s="34">
         <v>-3.0489999999999999</v>
       </c>
-      <c r="P98" s="27">
+      <c r="P98" s="34">
         <v>9.5500000000000007</v>
       </c>
-      <c r="Q98" s="27"/>
-      <c r="R98" s="27"/>
-      <c r="S98" s="27" t="s">
+      <c r="Q98" s="34"/>
+      <c r="R98" s="34"/>
+      <c r="S98" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T98" s="27">
+      <c r="T98" s="34">
         <v>2</v>
       </c>
-      <c r="U98" s="27">
-        <v>1</v>
-      </c>
-      <c r="V98" s="27">
+      <c r="U98" s="34">
+        <v>1</v>
+      </c>
+      <c r="V98" s="34">
         <v>-29.971</v>
       </c>
-      <c r="W98" s="27">
+      <c r="W98" s="34">
         <v>24.957999999999998</v>
       </c>
-      <c r="X98" s="27">
+      <c r="X98" s="34">
         <v>4.1580000000000004</v>
       </c>
-      <c r="Y98" s="27">
-        <v>0</v>
-      </c>
-      <c r="Z98" s="27"/>
-      <c r="AA98" s="27"/>
-      <c r="AB98" s="27"/>
-    </row>
-    <row r="99" spans="1:29" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A99" s="27" t="s">
+      <c r="Y98" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z98" s="34"/>
+      <c r="AA98" s="34"/>
+      <c r="AB98" s="34"/>
+    </row>
+    <row r="99" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A99" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B99" s="27"/>
-      <c r="C99" s="27" t="s">
+      <c r="B99" s="34"/>
+      <c r="C99" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="D99" s="27">
+      <c r="D99" s="34">
         <v>-3.0489999999999999</v>
       </c>
-      <c r="E99" s="27">
+      <c r="E99" s="34">
         <v>9.5500000000000007</v>
       </c>
-      <c r="F99" s="27">
+      <c r="F99" s="34">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G99" s="27">
+      <c r="G99" s="34">
         <v>0.5</v>
       </c>
-      <c r="H99" s="27">
+      <c r="H99" s="34">
         <v>-5.3490000000000002</v>
       </c>
-      <c r="I99" s="27">
+      <c r="I99" s="34">
         <v>-0.74900000000000011</v>
       </c>
-      <c r="J99" s="27">
+      <c r="J99" s="34">
         <v>9.8000000000000007</v>
       </c>
-      <c r="K99" s="27">
+      <c r="K99" s="34">
         <v>9.3000000000000007</v>
       </c>
-      <c r="L99" s="27"/>
-      <c r="M99" s="27">
-        <v>0</v>
-      </c>
-      <c r="N99" s="27">
-        <v>0</v>
-      </c>
-      <c r="O99" s="27">
+      <c r="L99" s="34"/>
+      <c r="M99" s="34">
+        <v>0</v>
+      </c>
+      <c r="N99" s="34">
+        <v>0</v>
+      </c>
+      <c r="O99" s="34">
         <v>-3.0489999999999999</v>
       </c>
-      <c r="P99" s="27">
+      <c r="P99" s="34">
         <v>9.5500000000000007</v>
       </c>
-      <c r="Q99" s="27"/>
-      <c r="R99" s="27"/>
-      <c r="S99" s="27" t="s">
+      <c r="Q99" s="34"/>
+      <c r="R99" s="34"/>
+      <c r="S99" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T99" s="27">
+      <c r="T99" s="34">
         <v>3</v>
       </c>
-      <c r="U99" s="27">
-        <v>1</v>
-      </c>
-      <c r="V99" s="27">
+      <c r="U99" s="34">
+        <v>1</v>
+      </c>
+      <c r="V99" s="34">
         <v>19.5</v>
       </c>
-      <c r="W99" s="27">
+      <c r="W99" s="34">
         <v>33.468000000000004</v>
       </c>
-      <c r="X99" s="27">
+      <c r="X99" s="34">
         <v>4.1500000000000004</v>
       </c>
-      <c r="Y99" s="27">
-        <v>0</v>
-      </c>
-      <c r="Z99" s="27"/>
-      <c r="AA99" s="27"/>
-      <c r="AB99" s="27"/>
+      <c r="Y99" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z99" s="34"/>
+      <c r="AA99" s="34"/>
+      <c r="AB99" s="34"/>
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
@@ -9634,78 +9635,77 @@
       <c r="AB119" s="1"/>
       <c r="AC119" s="1"/>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.45">
-      <c r="A120" s="1" t="s">
+    <row r="120" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A120" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1" t="s">
+      <c r="B120" s="34"/>
+      <c r="C120" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="D120" s="1">
-        <v>5.45</v>
-      </c>
-      <c r="E120" s="1">
+      <c r="D120" s="34">
+        <v>3.8</v>
+      </c>
+      <c r="E120" s="34">
         <v>10.25</v>
       </c>
-      <c r="F120" s="1">
-        <v>10.1</v>
-      </c>
-      <c r="G120" s="1">
+      <c r="F120" s="34">
+        <v>6.8</v>
+      </c>
+      <c r="G120" s="34">
         <v>1.5</v>
       </c>
-      <c r="H120" s="1">
-        <v>0.40000000000000041</v>
-      </c>
-      <c r="I120" s="1">
-        <v>10.5</v>
-      </c>
-      <c r="J120" s="1">
+      <c r="H120" s="34">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="I120" s="34">
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="J120" s="34">
         <v>11</v>
       </c>
-      <c r="K120" s="1">
+      <c r="K120" s="34">
         <v>9.5</v>
       </c>
-      <c r="L120" s="1"/>
-      <c r="M120" s="1">
-        <v>0</v>
-      </c>
-      <c r="N120" s="1">
-        <v>0</v>
-      </c>
-      <c r="O120" s="1">
-        <v>5.45</v>
-      </c>
-      <c r="P120" s="1">
+      <c r="L120" s="34"/>
+      <c r="M120" s="34">
+        <v>0</v>
+      </c>
+      <c r="N120" s="34">
+        <v>0</v>
+      </c>
+      <c r="O120" s="34">
+        <v>3.8</v>
+      </c>
+      <c r="P120" s="34">
         <v>10.25</v>
       </c>
-      <c r="Q120" s="1"/>
-      <c r="R120" s="1"/>
-      <c r="S120" s="1" t="s">
+      <c r="Q120" s="34"/>
+      <c r="R120" s="34"/>
+      <c r="S120" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T120" s="1">
+      <c r="T120" s="34">
         <v>4</v>
       </c>
-      <c r="U120" s="1">
+      <c r="U120" s="34">
         <v>2</v>
       </c>
-      <c r="V120" s="1">
+      <c r="V120" s="34">
         <v>-3.85</v>
       </c>
-      <c r="W120" s="1">
-        <v>0</v>
-      </c>
-      <c r="X120" s="1">
+      <c r="W120" s="34">
+        <v>0</v>
+      </c>
+      <c r="X120" s="34">
         <v>6.4</v>
       </c>
-      <c r="Y120" s="1">
+      <c r="Y120" s="34">
         <v>71.290000000000006</v>
       </c>
-      <c r="Z120" s="1"/>
-      <c r="AA120" s="1"/>
-      <c r="AB120" s="1"/>
-      <c r="AC120" s="1"/>
+      <c r="Z120" s="34"/>
+      <c r="AA120" s="34"/>
+      <c r="AB120" s="34"/>
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="s">
@@ -9782,149 +9782,149 @@
         <v>283</v>
       </c>
     </row>
-    <row r="122" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A122" s="29" t="s">
+    <row r="122" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A122" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B122" s="29"/>
-      <c r="C122" s="29" t="s">
+      <c r="B122" s="34"/>
+      <c r="C122" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="D122" s="29">
+      <c r="D122" s="34">
         <v>-1.65</v>
       </c>
-      <c r="E122" s="29">
+      <c r="E122" s="34">
         <v>-3.9</v>
       </c>
-      <c r="F122" s="29">
+      <c r="F122" s="34">
         <v>0.9</v>
       </c>
-      <c r="G122" s="29">
+      <c r="G122" s="34">
         <v>0.9</v>
       </c>
-      <c r="H122" s="29">
+      <c r="H122" s="34">
         <v>-2.1</v>
       </c>
-      <c r="I122" s="29">
+      <c r="I122" s="34">
         <v>-1.2</v>
       </c>
-      <c r="J122" s="29">
+      <c r="J122" s="34">
         <v>-3.45</v>
       </c>
-      <c r="K122" s="29">
+      <c r="K122" s="34">
         <v>-4.3499999999999996</v>
       </c>
-      <c r="L122" s="29"/>
-      <c r="M122" s="29">
-        <v>0</v>
-      </c>
-      <c r="N122" s="29">
-        <v>0</v>
-      </c>
-      <c r="O122" s="29">
+      <c r="L122" s="34"/>
+      <c r="M122" s="34">
+        <v>0</v>
+      </c>
+      <c r="N122" s="34">
+        <v>0</v>
+      </c>
+      <c r="O122" s="34">
         <v>-1.65</v>
       </c>
-      <c r="P122" s="29">
+      <c r="P122" s="34">
         <v>-3.9</v>
       </c>
-      <c r="Q122" s="29"/>
-      <c r="R122" s="29"/>
-      <c r="S122" s="29" t="s">
+      <c r="Q122" s="34"/>
+      <c r="R122" s="34"/>
+      <c r="S122" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T122" s="29">
+      <c r="T122" s="34">
         <v>11</v>
       </c>
-      <c r="U122" s="29">
-        <v>1</v>
-      </c>
-      <c r="V122" s="29">
+      <c r="U122" s="34">
+        <v>1</v>
+      </c>
+      <c r="V122" s="34">
         <v>14.5</v>
       </c>
-      <c r="W122" s="29">
+      <c r="W122" s="34">
         <v>35.945</v>
       </c>
-      <c r="X122" s="29">
-        <v>1</v>
-      </c>
-      <c r="Y122" s="29">
-        <v>0</v>
-      </c>
-      <c r="Z122" s="29"/>
-      <c r="AA122" s="29"/>
-      <c r="AB122" s="29"/>
-    </row>
-    <row r="123" spans="1:29" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A123" s="29" t="s">
+      <c r="X122" s="34">
+        <v>1</v>
+      </c>
+      <c r="Y122" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z122" s="34"/>
+      <c r="AA122" s="34"/>
+      <c r="AB122" s="34"/>
+    </row>
+    <row r="123" spans="1:29" s="33" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A123" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="B123" s="29"/>
-      <c r="C123" s="29" t="s">
+      <c r="B123" s="34"/>
+      <c r="C123" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="D123" s="29">
+      <c r="D123" s="34">
         <v>-1.65</v>
       </c>
-      <c r="E123" s="29">
+      <c r="E123" s="34">
         <v>-3.9</v>
       </c>
-      <c r="F123" s="29">
+      <c r="F123" s="34">
         <v>0.9</v>
       </c>
-      <c r="G123" s="29">
+      <c r="G123" s="34">
         <v>0.9</v>
       </c>
-      <c r="H123" s="29">
+      <c r="H123" s="34">
         <v>-2.1</v>
       </c>
-      <c r="I123" s="29">
+      <c r="I123" s="34">
         <v>-1.2</v>
       </c>
-      <c r="J123" s="29">
+      <c r="J123" s="34">
         <v>-3.45</v>
       </c>
-      <c r="K123" s="29">
+      <c r="K123" s="34">
         <v>-4.3499999999999996</v>
       </c>
-      <c r="L123" s="29"/>
-      <c r="M123" s="29">
-        <v>0</v>
-      </c>
-      <c r="N123" s="29">
-        <v>0</v>
-      </c>
-      <c r="O123" s="29">
+      <c r="L123" s="34"/>
+      <c r="M123" s="34">
+        <v>0</v>
+      </c>
+      <c r="N123" s="34">
+        <v>0</v>
+      </c>
+      <c r="O123" s="34">
         <v>-1.65</v>
       </c>
-      <c r="P123" s="29">
+      <c r="P123" s="34">
         <v>-3.9</v>
       </c>
-      <c r="Q123" s="29"/>
-      <c r="R123" s="29"/>
-      <c r="S123" s="29" t="s">
+      <c r="Q123" s="34"/>
+      <c r="R123" s="34"/>
+      <c r="S123" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="T123" s="29">
+      <c r="T123" s="34">
         <v>11</v>
       </c>
-      <c r="U123" s="29">
-        <v>1</v>
-      </c>
-      <c r="V123" s="29">
+      <c r="U123" s="34">
+        <v>1</v>
+      </c>
+      <c r="V123" s="34">
         <v>-22.2</v>
       </c>
-      <c r="W123" s="29">
+      <c r="W123" s="34">
         <v>35.945</v>
       </c>
-      <c r="X123" s="29">
-        <v>1</v>
-      </c>
-      <c r="Y123" s="29">
-        <v>0</v>
-      </c>
-      <c r="Z123" s="29"/>
-      <c r="AA123" s="29"/>
-      <c r="AB123" s="29"/>
+      <c r="X123" s="34">
+        <v>1</v>
+      </c>
+      <c r="Y123" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z123" s="34"/>
+      <c r="AA123" s="34"/>
+      <c r="AB123" s="34"/>
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A124" s="1" t="s">
@@ -12441,18 +12441,18 @@
       <c r="A1" s="3"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="27" t="s">
         <v>268</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="31" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="27" t="s">
         <v>269</v>
       </c>
-      <c r="I1" s="32"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
         <v>270</v>
@@ -28616,18 +28616,18 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="31" t="s">
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="32"/>
+      <c r="AA1" s="28"/>
       <c r="AB1" s="1"/>
       <c r="AE1" s="15"/>
       <c r="AF1" s="16"/>
@@ -28637,10 +28637,10 @@
       <c r="AJ1" s="16"/>
       <c r="AK1" s="16"/>
       <c r="AL1" s="16"/>
-      <c r="AM1" s="33" t="s">
+      <c r="AM1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="AN1" s="34"/>
+      <c r="AN1" s="30"/>
       <c r="AO1" s="16"/>
       <c r="AP1" s="18"/>
       <c r="AQ1" s="18"/>
@@ -28651,74 +28651,74 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="31" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="31" t="s">
+      <c r="G2" s="28"/>
+      <c r="H2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="32"/>
-      <c r="O2" s="31" t="s">
+      <c r="N2" s="28"/>
+      <c r="O2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="32"/>
+      <c r="P2" s="28"/>
       <c r="Q2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="32"/>
-      <c r="V2" s="31" t="s">
+      <c r="U2" s="28"/>
+      <c r="V2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="32"/>
-      <c r="X2" s="31" t="s">
+      <c r="W2" s="28"/>
+      <c r="X2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="31" t="s">
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AA2" s="32"/>
+      <c r="AA2" s="28"/>
       <c r="AB2" s="1"/>
       <c r="AE2" s="15"/>
       <c r="AF2" s="16"/>
-      <c r="AG2" s="33" t="s">
+      <c r="AG2" s="29" t="s">
         <v>287</v>
       </c>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
       <c r="AK2" s="16"/>
       <c r="AL2" s="16"/>
-      <c r="AM2" s="33" t="s">
+      <c r="AM2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="AN2" s="34"/>
+      <c r="AN2" s="30"/>
       <c r="AO2" s="16"/>
-      <c r="AP2" s="35" t="s">
+      <c r="AP2" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="AQ2" s="36"/>
-      <c r="AR2" s="35" t="s">
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="AS2" s="36"/>
+      <c r="AS2" s="32"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
giving the cell drop a second run
</commit_message>
<xml_diff>
--- a/masks/code/TKIDModule_spreadsheet_20200602_AW_CF.xlsx
+++ b/masks/code/TKIDModule_spreadsheet_20200602_AW_CF.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Patches" sheetId="1" r:id="rId1"/>
@@ -878,9 +878,6 @@
     <t>Drop R1C1, R1C3, R1C5, R2C2, R2C4</t>
   </si>
   <si>
-    <t>Drop R1C1, R1C2, R1C9, R2C1, R2C8, R2C9. R3C9, R4C1, R7C9, R8C1, R11C9, R12C1, R15C1, R15C9, R16C1, R16C9</t>
-  </si>
-  <si>
     <t>Parameter:Auto align: offset=Wafer Shift = (Mask shift - Cell Shift)</t>
   </si>
   <si>
@@ -894,6 +891,9 @@
   </si>
   <si>
     <t>capacitor_Nbpatch</t>
+  </si>
+  <si>
+    <t>Drop R1C1, R2C1, R4C1, R8C1, R12C1, R15C1, R16C1, R1C2, R8C2, R9C1, R9C2, R9C3, R9C7, R9C11, R9C15, R9C16</t>
   </si>
 </sst>
 </file>
@@ -1366,9 +1366,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AC157"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC14" sqref="AC14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC67" sqref="AC67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4053,7 +4053,7 @@
         <v>52</v>
       </c>
       <c r="AC44" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.45">
@@ -5603,8 +5603,8 @@
       <c r="AB65" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AC65" s="21" t="s">
-        <v>285</v>
+      <c r="AC65" s="16" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="66" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.45">
@@ -5753,8 +5753,8 @@
       <c r="AB67" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AC67" s="21" t="s">
-        <v>285</v>
+      <c r="AC67" s="16" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.45">
@@ -5909,7 +5909,7 @@
       </c>
       <c r="B70" s="21"/>
       <c r="C70" s="21" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D70" s="21">
         <v>-5.4</v>
@@ -6350,7 +6350,7 @@
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D76" s="21">
         <v>-6.39</v>
@@ -12339,7 +12339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB518"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -13239,7 +13239,7 @@
     <row r="21" spans="1:28" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>66</v>
@@ -29245,9 +29245,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87:XFD87"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC143" sqref="AC143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29711,7 +29711,7 @@
       <c r="Q15" s="21"/>
       <c r="R15" s="21"/>
       <c r="S15" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T15" s="21">
         <v>1</v>
@@ -29783,7 +29783,7 @@
       <c r="Q16" s="21"/>
       <c r="R16" s="21"/>
       <c r="S16" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T16" s="21">
         <v>1</v>
@@ -29856,7 +29856,7 @@
       <c r="Q17" s="21"/>
       <c r="R17" s="21"/>
       <c r="S17" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T17" s="21">
         <v>1</v>
@@ -29930,7 +29930,7 @@
       <c r="Q18" s="21"/>
       <c r="R18" s="21"/>
       <c r="S18" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T18" s="21">
         <v>1</v>
@@ -30004,7 +30004,7 @@
       <c r="Q19" s="21"/>
       <c r="R19" s="21"/>
       <c r="S19" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T19" s="21">
         <v>1</v>
@@ -30078,7 +30078,7 @@
       <c r="Q20" s="21"/>
       <c r="R20" s="21"/>
       <c r="S20" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T20" s="21">
         <v>1</v>
@@ -30152,7 +30152,7 @@
       <c r="Q21" s="21"/>
       <c r="R21" s="21"/>
       <c r="S21" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T21" s="21">
         <v>1</v>
@@ -30226,7 +30226,7 @@
       <c r="Q22" s="21"/>
       <c r="R22" s="21"/>
       <c r="S22" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T22" s="21">
         <v>1</v>
@@ -30300,7 +30300,7 @@
       <c r="Q23" s="21"/>
       <c r="R23" s="21"/>
       <c r="S23" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T23" s="21">
         <v>1</v>
@@ -30374,7 +30374,7 @@
       <c r="Q24" s="21"/>
       <c r="R24" s="21"/>
       <c r="S24" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T24" s="21">
         <v>1</v>
@@ -30448,7 +30448,7 @@
       <c r="Q25" s="21"/>
       <c r="R25" s="21"/>
       <c r="S25" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T25" s="21">
         <v>1</v>
@@ -30522,7 +30522,7 @@
       <c r="Q26" s="21"/>
       <c r="R26" s="21"/>
       <c r="S26" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T26" s="21">
         <v>1</v>
@@ -30596,7 +30596,7 @@
       <c r="Q27" s="21"/>
       <c r="R27" s="21"/>
       <c r="S27" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T27" s="21">
         <v>1</v>
@@ -30670,7 +30670,7 @@
       <c r="Q28" s="21"/>
       <c r="R28" s="21"/>
       <c r="S28" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T28" s="21">
         <v>1</v>
@@ -30744,7 +30744,7 @@
       <c r="Q29" s="21"/>
       <c r="R29" s="21"/>
       <c r="S29" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T29" s="21">
         <v>1</v>
@@ -30818,7 +30818,7 @@
       <c r="Q30" s="21"/>
       <c r="R30" s="21"/>
       <c r="S30" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T30" s="21">
         <v>1</v>
@@ -30892,7 +30892,7 @@
       <c r="Q31" s="21"/>
       <c r="R31" s="21"/>
       <c r="S31" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T31" s="21">
         <v>1</v>
@@ -30966,7 +30966,7 @@
       <c r="Q32" s="21"/>
       <c r="R32" s="21"/>
       <c r="S32" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T32" s="21">
         <v>1</v>
@@ -31040,7 +31040,7 @@
       <c r="Q33" s="21"/>
       <c r="R33" s="21"/>
       <c r="S33" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T33" s="21">
         <v>1</v>
@@ -31114,7 +31114,7 @@
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
       <c r="S34" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T34" s="21">
         <v>1</v>
@@ -31188,7 +31188,7 @@
       <c r="Q35" s="21"/>
       <c r="R35" s="21"/>
       <c r="S35" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T35" s="21">
         <v>1</v>
@@ -31262,7 +31262,7 @@
       <c r="Q36" s="21"/>
       <c r="R36" s="21"/>
       <c r="S36" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T36" s="21">
         <v>1</v>
@@ -31336,7 +31336,7 @@
       <c r="Q37" s="21"/>
       <c r="R37" s="21"/>
       <c r="S37" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T37" s="21">
         <v>1</v>
@@ -31410,7 +31410,7 @@
       <c r="Q38" s="21"/>
       <c r="R38" s="21"/>
       <c r="S38" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T38" s="21">
         <v>1</v>
@@ -31484,7 +31484,7 @@
       <c r="Q39" s="21"/>
       <c r="R39" s="21"/>
       <c r="S39" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T39" s="21">
         <v>1</v>
@@ -31558,7 +31558,7 @@
       <c r="Q40" s="21"/>
       <c r="R40" s="21"/>
       <c r="S40" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T40" s="21">
         <v>1</v>
@@ -31632,7 +31632,7 @@
       <c r="Q41" s="21"/>
       <c r="R41" s="21"/>
       <c r="S41" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T41" s="21">
         <v>1</v>
@@ -31706,7 +31706,7 @@
       <c r="Q42" s="21"/>
       <c r="R42" s="21"/>
       <c r="S42" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T42" s="21">
         <v>1</v>
@@ -31780,7 +31780,7 @@
       <c r="Q43" s="21"/>
       <c r="R43" s="21"/>
       <c r="S43" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T43" s="21">
         <v>1</v>
@@ -31854,7 +31854,7 @@
       <c r="Q44" s="21"/>
       <c r="R44" s="21"/>
       <c r="S44" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T44" s="21">
         <v>1</v>
@@ -31928,7 +31928,7 @@
       <c r="Q45" s="21"/>
       <c r="R45" s="21"/>
       <c r="S45" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T45" s="21">
         <v>1</v>
@@ -32002,7 +32002,7 @@
       <c r="Q46" s="21"/>
       <c r="R46" s="21"/>
       <c r="S46" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T46" s="21">
         <v>1</v>
@@ -32076,7 +32076,7 @@
       <c r="Q47" s="21"/>
       <c r="R47" s="21"/>
       <c r="S47" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T47" s="21">
         <v>1</v>
@@ -32150,7 +32150,7 @@
       <c r="Q48" s="21"/>
       <c r="R48" s="21"/>
       <c r="S48" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T48" s="21">
         <v>1</v>
@@ -32224,7 +32224,7 @@
       <c r="Q49" s="21"/>
       <c r="R49" s="21"/>
       <c r="S49" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T49" s="21">
         <v>1</v>
@@ -32298,7 +32298,7 @@
       <c r="Q50" s="21"/>
       <c r="R50" s="21"/>
       <c r="S50" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T50" s="21">
         <v>1</v>
@@ -32372,7 +32372,7 @@
       <c r="Q51" s="21"/>
       <c r="R51" s="21"/>
       <c r="S51" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T51" s="21">
         <v>1</v>
@@ -32446,7 +32446,7 @@
       <c r="Q52" s="21"/>
       <c r="R52" s="21"/>
       <c r="S52" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T52" s="21">
         <v>1</v>
@@ -32520,7 +32520,7 @@
       <c r="Q53" s="21"/>
       <c r="R53" s="21"/>
       <c r="S53" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T53" s="21">
         <v>1</v>
@@ -32594,7 +32594,7 @@
       <c r="Q54" s="21"/>
       <c r="R54" s="21"/>
       <c r="S54" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T54" s="21">
         <v>1</v>
@@ -32668,7 +32668,7 @@
       <c r="Q55" s="21"/>
       <c r="R55" s="21"/>
       <c r="S55" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T55" s="21">
         <v>1</v>
@@ -32742,7 +32742,7 @@
       <c r="Q56" s="21"/>
       <c r="R56" s="21"/>
       <c r="S56" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T56" s="21">
         <v>1</v>
@@ -32816,7 +32816,7 @@
       <c r="Q57" s="21"/>
       <c r="R57" s="21"/>
       <c r="S57" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T57" s="21">
         <v>1</v>
@@ -32890,7 +32890,7 @@
       <c r="Q58" s="21"/>
       <c r="R58" s="21"/>
       <c r="S58" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T58" s="21">
         <v>1</v>
@@ -32964,7 +32964,7 @@
       <c r="Q59" s="21"/>
       <c r="R59" s="21"/>
       <c r="S59" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T59" s="21">
         <v>1</v>
@@ -33038,7 +33038,7 @@
       <c r="Q60" s="21"/>
       <c r="R60" s="21"/>
       <c r="S60" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T60" s="21">
         <v>1</v>
@@ -33112,7 +33112,7 @@
       <c r="Q61" s="21"/>
       <c r="R61" s="21"/>
       <c r="S61" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T61" s="21">
         <v>1</v>
@@ -33186,7 +33186,7 @@
       <c r="Q62" s="21"/>
       <c r="R62" s="21"/>
       <c r="S62" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T62" s="21">
         <v>1</v>
@@ -33260,7 +33260,7 @@
       <c r="Q63" s="21"/>
       <c r="R63" s="21"/>
       <c r="S63" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T63" s="21">
         <v>1</v>
@@ -33334,7 +33334,7 @@
       <c r="Q64" s="21"/>
       <c r="R64" s="21"/>
       <c r="S64" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T64" s="21">
         <v>1</v>
@@ -33408,7 +33408,7 @@
       <c r="Q65" s="21"/>
       <c r="R65" s="21"/>
       <c r="S65" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T65" s="21">
         <v>1</v>
@@ -33482,7 +33482,7 @@
       <c r="Q66" s="21"/>
       <c r="R66" s="21"/>
       <c r="S66" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T66" s="21">
         <v>1</v>
@@ -33556,7 +33556,7 @@
       <c r="Q67" s="21"/>
       <c r="R67" s="21"/>
       <c r="S67" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T67" s="21">
         <v>1</v>
@@ -33630,7 +33630,7 @@
       <c r="Q68" s="21"/>
       <c r="R68" s="21"/>
       <c r="S68" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T68" s="21">
         <v>1</v>
@@ -33704,7 +33704,7 @@
       <c r="Q69" s="21"/>
       <c r="R69" s="21"/>
       <c r="S69" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T69" s="21">
         <v>1</v>
@@ -33778,7 +33778,7 @@
       <c r="Q70" s="21"/>
       <c r="R70" s="21"/>
       <c r="S70" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T70" s="21">
         <v>1</v>
@@ -33852,7 +33852,7 @@
       <c r="Q71" s="21"/>
       <c r="R71" s="21"/>
       <c r="S71" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T71" s="21">
         <v>1</v>
@@ -33926,7 +33926,7 @@
       <c r="Q72" s="21"/>
       <c r="R72" s="21"/>
       <c r="S72" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T72" s="21">
         <v>1</v>
@@ -34000,7 +34000,7 @@
       <c r="Q73" s="21"/>
       <c r="R73" s="21"/>
       <c r="S73" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T73" s="21">
         <v>1</v>
@@ -34074,7 +34074,7 @@
       <c r="Q74" s="21"/>
       <c r="R74" s="21"/>
       <c r="S74" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T74" s="21">
         <v>1</v>
@@ -34148,7 +34148,7 @@
       <c r="Q75" s="21"/>
       <c r="R75" s="21"/>
       <c r="S75" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T75" s="21">
         <v>1</v>
@@ -34222,7 +34222,7 @@
       <c r="Q76" s="21"/>
       <c r="R76" s="21"/>
       <c r="S76" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T76" s="21">
         <v>1</v>
@@ -34296,7 +34296,7 @@
       <c r="Q77" s="21"/>
       <c r="R77" s="21"/>
       <c r="S77" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T77" s="21">
         <v>1</v>
@@ -34370,7 +34370,7 @@
       <c r="Q78" s="21"/>
       <c r="R78" s="21"/>
       <c r="S78" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T78" s="21">
         <v>1</v>
@@ -34444,7 +34444,7 @@
       <c r="Q79" s="21"/>
       <c r="R79" s="21"/>
       <c r="S79" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T79" s="21">
         <v>1</v>
@@ -34518,7 +34518,7 @@
       <c r="Q80" s="21"/>
       <c r="R80" s="21"/>
       <c r="S80" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T80" s="21">
         <v>1</v>
@@ -34592,7 +34592,7 @@
       <c r="Q81" s="21"/>
       <c r="R81" s="21"/>
       <c r="S81" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T81" s="21">
         <v>1</v>
@@ -34666,7 +34666,7 @@
       <c r="Q82" s="21"/>
       <c r="R82" s="21"/>
       <c r="S82" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T82" s="21">
         <v>1</v>
@@ -34740,7 +34740,7 @@
       <c r="Q83" s="21"/>
       <c r="R83" s="21"/>
       <c r="S83" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T83" s="21">
         <v>1</v>
@@ -34814,7 +34814,7 @@
       <c r="Q84" s="21"/>
       <c r="R84" s="21"/>
       <c r="S84" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T84" s="21">
         <v>1</v>
@@ -34888,7 +34888,7 @@
       <c r="Q85" s="21"/>
       <c r="R85" s="21"/>
       <c r="S85" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T85" s="21">
         <v>1</v>
@@ -34962,7 +34962,7 @@
       <c r="Q86" s="21"/>
       <c r="R86" s="21"/>
       <c r="S86" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T86" s="21">
         <v>1</v>
@@ -35036,7 +35036,7 @@
       <c r="Q87" s="21"/>
       <c r="R87" s="21"/>
       <c r="S87" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T87" s="21">
         <v>1</v>
@@ -35110,7 +35110,7 @@
       <c r="Q88" s="21"/>
       <c r="R88" s="21"/>
       <c r="S88" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T88" s="21">
         <v>1</v>
@@ -35184,7 +35184,7 @@
       <c r="Q89" s="21"/>
       <c r="R89" s="21"/>
       <c r="S89" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T89" s="21">
         <v>1</v>
@@ -35258,7 +35258,7 @@
       <c r="Q90" s="21"/>
       <c r="R90" s="21"/>
       <c r="S90" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T90" s="21">
         <v>1</v>
@@ -35332,7 +35332,7 @@
       <c r="Q91" s="21"/>
       <c r="R91" s="21"/>
       <c r="S91" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T91" s="21">
         <v>1</v>
@@ -35406,7 +35406,7 @@
       <c r="Q92" s="21"/>
       <c r="R92" s="21"/>
       <c r="S92" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T92" s="21">
         <v>1</v>
@@ -35480,7 +35480,7 @@
       <c r="Q93" s="21"/>
       <c r="R93" s="21"/>
       <c r="S93" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T93" s="21">
         <v>1</v>
@@ -35554,7 +35554,7 @@
       <c r="Q94" s="21"/>
       <c r="R94" s="21"/>
       <c r="S94" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T94" s="21">
         <v>1</v>
@@ -35628,7 +35628,7 @@
       <c r="Q95" s="21"/>
       <c r="R95" s="21"/>
       <c r="S95" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T95" s="21">
         <v>1</v>
@@ -35702,7 +35702,7 @@
       <c r="Q96" s="21"/>
       <c r="R96" s="21"/>
       <c r="S96" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T96" s="21">
         <v>1</v>
@@ -35776,7 +35776,7 @@
       <c r="Q97" s="21"/>
       <c r="R97" s="21"/>
       <c r="S97" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T97" s="21">
         <v>1</v>
@@ -35850,7 +35850,7 @@
       <c r="Q98" s="21"/>
       <c r="R98" s="21"/>
       <c r="S98" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T98" s="21">
         <v>1</v>
@@ -35924,7 +35924,7 @@
       <c r="Q99" s="21"/>
       <c r="R99" s="21"/>
       <c r="S99" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T99" s="21">
         <v>1</v>
@@ -35998,7 +35998,7 @@
       <c r="Q100" s="21"/>
       <c r="R100" s="21"/>
       <c r="S100" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T100" s="21">
         <v>1</v>
@@ -36072,7 +36072,7 @@
       <c r="Q101" s="21"/>
       <c r="R101" s="21"/>
       <c r="S101" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T101" s="21">
         <v>1</v>
@@ -36146,7 +36146,7 @@
       <c r="Q102" s="21"/>
       <c r="R102" s="21"/>
       <c r="S102" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T102" s="21">
         <v>1</v>
@@ -36220,7 +36220,7 @@
       <c r="Q103" s="21"/>
       <c r="R103" s="21"/>
       <c r="S103" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T103" s="21">
         <v>1</v>
@@ -36294,7 +36294,7 @@
       <c r="Q104" s="21"/>
       <c r="R104" s="21"/>
       <c r="S104" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T104" s="21">
         <v>1</v>
@@ -36368,7 +36368,7 @@
       <c r="Q105" s="21"/>
       <c r="R105" s="21"/>
       <c r="S105" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T105" s="21">
         <v>1</v>
@@ -36442,7 +36442,7 @@
       <c r="Q106" s="21"/>
       <c r="R106" s="21"/>
       <c r="S106" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T106" s="21">
         <v>1</v>
@@ -36516,7 +36516,7 @@
       <c r="Q107" s="21"/>
       <c r="R107" s="21"/>
       <c r="S107" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T107" s="21">
         <v>1</v>
@@ -36590,7 +36590,7 @@
       <c r="Q108" s="21"/>
       <c r="R108" s="21"/>
       <c r="S108" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T108" s="21">
         <v>1</v>
@@ -36664,7 +36664,7 @@
       <c r="Q109" s="21"/>
       <c r="R109" s="21"/>
       <c r="S109" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T109" s="21">
         <v>1</v>
@@ -36738,7 +36738,7 @@
       <c r="Q110" s="21"/>
       <c r="R110" s="21"/>
       <c r="S110" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T110" s="21">
         <v>1</v>
@@ -36812,7 +36812,7 @@
       <c r="Q111" s="21"/>
       <c r="R111" s="21"/>
       <c r="S111" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T111" s="21">
         <v>1</v>
@@ -36886,7 +36886,7 @@
       <c r="Q112" s="21"/>
       <c r="R112" s="21"/>
       <c r="S112" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T112" s="21">
         <v>1</v>
@@ -36960,7 +36960,7 @@
       <c r="Q113" s="21"/>
       <c r="R113" s="21"/>
       <c r="S113" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T113" s="21">
         <v>1</v>
@@ -37034,7 +37034,7 @@
       <c r="Q114" s="21"/>
       <c r="R114" s="21"/>
       <c r="S114" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T114" s="21">
         <v>1</v>
@@ -37108,7 +37108,7 @@
       <c r="Q115" s="21"/>
       <c r="R115" s="21"/>
       <c r="S115" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T115" s="21">
         <v>1</v>
@@ -37182,7 +37182,7 @@
       <c r="Q116" s="21"/>
       <c r="R116" s="21"/>
       <c r="S116" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T116" s="21">
         <v>1</v>
@@ -37256,7 +37256,7 @@
       <c r="Q117" s="21"/>
       <c r="R117" s="21"/>
       <c r="S117" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T117" s="21">
         <v>1</v>
@@ -37330,7 +37330,7 @@
       <c r="Q118" s="21"/>
       <c r="R118" s="21"/>
       <c r="S118" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T118" s="21">
         <v>1</v>
@@ -37404,7 +37404,7 @@
       <c r="Q119" s="21"/>
       <c r="R119" s="21"/>
       <c r="S119" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T119" s="21">
         <v>1</v>
@@ -37478,7 +37478,7 @@
       <c r="Q120" s="21"/>
       <c r="R120" s="21"/>
       <c r="S120" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T120" s="21">
         <v>1</v>
@@ -37552,7 +37552,7 @@
       <c r="Q121" s="21"/>
       <c r="R121" s="21"/>
       <c r="S121" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T121" s="21">
         <v>1</v>
@@ -37626,7 +37626,7 @@
       <c r="Q122" s="21"/>
       <c r="R122" s="21"/>
       <c r="S122" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T122" s="21">
         <v>1</v>
@@ -37700,7 +37700,7 @@
       <c r="Q123" s="21"/>
       <c r="R123" s="21"/>
       <c r="S123" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T123" s="21">
         <v>1</v>
@@ -37774,7 +37774,7 @@
       <c r="Q124" s="21"/>
       <c r="R124" s="21"/>
       <c r="S124" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T124" s="21">
         <v>1</v>
@@ -37848,7 +37848,7 @@
       <c r="Q125" s="21"/>
       <c r="R125" s="21"/>
       <c r="S125" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T125" s="21">
         <v>1</v>
@@ -37922,7 +37922,7 @@
       <c r="Q126" s="21"/>
       <c r="R126" s="21"/>
       <c r="S126" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T126" s="21">
         <v>1</v>
@@ -37996,7 +37996,7 @@
       <c r="Q127" s="21"/>
       <c r="R127" s="21"/>
       <c r="S127" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T127" s="21">
         <v>1</v>
@@ -38070,7 +38070,7 @@
       <c r="Q128" s="21"/>
       <c r="R128" s="21"/>
       <c r="S128" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T128" s="21">
         <v>1</v>
@@ -38144,7 +38144,7 @@
       <c r="Q129" s="21"/>
       <c r="R129" s="21"/>
       <c r="S129" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T129" s="21">
         <v>1</v>
@@ -38218,7 +38218,7 @@
       <c r="Q130" s="21"/>
       <c r="R130" s="21"/>
       <c r="S130" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T130" s="21">
         <v>1</v>
@@ -38292,7 +38292,7 @@
       <c r="Q131" s="21"/>
       <c r="R131" s="21"/>
       <c r="S131" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T131" s="21">
         <v>1</v>
@@ -38366,7 +38366,7 @@
       <c r="Q132" s="21"/>
       <c r="R132" s="21"/>
       <c r="S132" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T132" s="21">
         <v>1</v>
@@ -38440,7 +38440,7 @@
       <c r="Q133" s="21"/>
       <c r="R133" s="21"/>
       <c r="S133" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T133" s="21">
         <v>1</v>
@@ -38514,7 +38514,7 @@
       <c r="Q134" s="21"/>
       <c r="R134" s="21"/>
       <c r="S134" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T134" s="21">
         <v>1</v>
@@ -38588,7 +38588,7 @@
       <c r="Q135" s="21"/>
       <c r="R135" s="21"/>
       <c r="S135" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T135" s="21">
         <v>1</v>
@@ -38662,7 +38662,7 @@
       <c r="Q136" s="21"/>
       <c r="R136" s="21"/>
       <c r="S136" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T136" s="21">
         <v>1</v>
@@ -38736,7 +38736,7 @@
       <c r="Q137" s="21"/>
       <c r="R137" s="21"/>
       <c r="S137" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T137" s="21">
         <v>1</v>
@@ -38810,7 +38810,7 @@
       <c r="Q138" s="21"/>
       <c r="R138" s="21"/>
       <c r="S138" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T138" s="21">
         <v>1</v>
@@ -38884,7 +38884,7 @@
       <c r="Q139" s="21"/>
       <c r="R139" s="21"/>
       <c r="S139" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T139" s="21">
         <v>1</v>
@@ -38958,7 +38958,7 @@
       <c r="Q140" s="21"/>
       <c r="R140" s="21"/>
       <c r="S140" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T140" s="21">
         <v>1</v>
@@ -39032,7 +39032,7 @@
       <c r="Q141" s="21"/>
       <c r="R141" s="21"/>
       <c r="S141" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T141" s="21">
         <v>1</v>
@@ -39106,7 +39106,7 @@
       <c r="Q142" s="21"/>
       <c r="R142" s="21"/>
       <c r="S142" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T142" s="21">
         <v>1</v>
@@ -39136,7 +39136,7 @@
       </c>
       <c r="B143" s="21"/>
       <c r="C143" s="21" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D143" s="21">
         <v>-1.5</v>
@@ -39178,7 +39178,7 @@
       <c r="Q143" s="21"/>
       <c r="R143" s="21"/>
       <c r="S143" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T143" s="21">
         <v>9</v>
@@ -39203,8 +39203,8 @@
       <c r="AB143" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="AC143" s="21" t="s">
-        <v>285</v>
+      <c r="AC143" s="16" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="144" spans="1:45" x14ac:dyDescent="0.45">
@@ -39277,7 +39277,7 @@
     </row>
     <row r="148" spans="1:45" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A148" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B148" s="10"/>
       <c r="C148" s="10"/>

</xml_diff>